<commit_message>
Implemented full feeder 4 model
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
   <si>
     <t>Stim.CB.CB401</t>
   </si>
@@ -67,6 +67,51 @@
   </si>
   <si>
     <t>];</t>
+  </si>
+  <si>
+    <t>Stim.PV.p</t>
+  </si>
+  <si>
+    <t>Stim.PV.Ena</t>
+  </si>
+  <si>
+    <t>GenP</t>
+  </si>
+  <si>
+    <t>ESS2P</t>
+  </si>
+  <si>
+    <t>PVP</t>
+  </si>
+  <si>
+    <t>Loads</t>
+  </si>
+  <si>
+    <t>Stim.CB.CB405</t>
+  </si>
+  <si>
+    <t>Stim.CB.CB407</t>
+  </si>
+  <si>
+    <t>Stim.CB.CB408</t>
+  </si>
+  <si>
+    <t>Stim.CB.CB409</t>
+  </si>
+  <si>
+    <t>Stim.CB.CB411</t>
+  </si>
+  <si>
+    <t>Stim.CB.CB412</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>MCB</t>
+  </si>
+  <si>
+    <t>GenQ</t>
   </si>
 </sst>
 </file>
@@ -436,165 +481,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL19"/>
+  <dimension ref="A1:AM39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL15" sqref="A2:AL15"/>
+      <selection activeCell="AM23" sqref="A2:AM23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.109375" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="42" width="4.77734375" customWidth="1"/>
+    <col min="3" max="43" width="4.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="C1" s="1">
         <v>0</v>
       </c>
       <c r="D1">
         <f>C1+C1-B1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1">
         <f>D1+D1-C1</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F1">
-        <f t="shared" ref="F1:Y1" si="0">E1+E1-D1</f>
-        <v>3</v>
+        <f t="shared" ref="F1:I1" si="0">E1+E1-D1</f>
+        <v>9</v>
       </c>
       <c r="G1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="J1">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f t="shared" ref="J1" si="1">I1+I1-H1</f>
+        <v>21</v>
       </c>
       <c r="K1">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" ref="K1" si="2">J1+J1-I1</f>
+        <v>24</v>
       </c>
       <c r="L1">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" ref="L1" si="3">K1+K1-J1</f>
+        <v>27</v>
       </c>
       <c r="M1">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" ref="M1" si="4">L1+L1-K1</f>
+        <v>30</v>
       </c>
       <c r="N1">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" ref="N1" si="5">M1+M1-L1</f>
+        <v>33</v>
       </c>
       <c r="O1">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f t="shared" ref="O1" si="6">N1+N1-M1</f>
+        <v>36</v>
       </c>
       <c r="P1">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f t="shared" ref="P1" si="7">O1+O1-N1</f>
+        <v>39</v>
       </c>
       <c r="Q1">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f t="shared" ref="Q1" si="8">P1+P1-O1</f>
+        <v>42</v>
       </c>
       <c r="R1">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f t="shared" ref="R1" si="9">Q1+Q1-P1</f>
+        <v>45</v>
       </c>
       <c r="S1">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f t="shared" ref="S1" si="10">R1+R1-Q1</f>
+        <v>48</v>
       </c>
       <c r="T1">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f t="shared" ref="T1" si="11">S1+S1-R1</f>
+        <v>51</v>
       </c>
       <c r="U1">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f t="shared" ref="U1" si="12">T1+T1-S1</f>
+        <v>54</v>
       </c>
       <c r="V1">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f t="shared" ref="V1" si="13">U1+U1-T1</f>
+        <v>57</v>
       </c>
       <c r="W1">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f t="shared" ref="W1" si="14">V1+V1-U1</f>
+        <v>60</v>
       </c>
       <c r="X1">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <f t="shared" ref="X1" si="15">W1+W1-V1</f>
+        <v>63</v>
       </c>
       <c r="Y1">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <f t="shared" ref="Y1" si="16">X1+X1-W1</f>
+        <v>66</v>
       </c>
       <c r="Z1">
-        <f t="shared" ref="Z1" si="1">Y1+Y1-X1</f>
-        <v>23</v>
+        <f t="shared" ref="Z1" si="17">Y1+Y1-X1</f>
+        <v>69</v>
       </c>
       <c r="AA1">
-        <f t="shared" ref="AA1" si="2">Z1+Z1-Y1</f>
-        <v>24</v>
+        <f t="shared" ref="AA1" si="18">Z1+Z1-Y1</f>
+        <v>72</v>
       </c>
       <c r="AB1">
-        <f t="shared" ref="AB1" si="3">AA1+AA1-Z1</f>
-        <v>25</v>
+        <f t="shared" ref="AB1" si="19">AA1+AA1-Z1</f>
+        <v>75</v>
       </c>
       <c r="AC1">
-        <f t="shared" ref="AC1" si="4">AB1+AB1-AA1</f>
-        <v>26</v>
+        <f t="shared" ref="AC1" si="20">AB1+AB1-AA1</f>
+        <v>78</v>
       </c>
       <c r="AD1">
-        <f t="shared" ref="AD1" si="5">AC1+AC1-AB1</f>
-        <v>27</v>
+        <f t="shared" ref="AD1" si="21">AC1+AC1-AB1</f>
+        <v>81</v>
       </c>
       <c r="AE1">
-        <f t="shared" ref="AE1" si="6">AD1+AD1-AC1</f>
-        <v>28</v>
+        <f t="shared" ref="AE1" si="22">AD1+AD1-AC1</f>
+        <v>84</v>
       </c>
       <c r="AF1">
-        <f t="shared" ref="AF1" si="7">AE1+AE1-AD1</f>
-        <v>29</v>
+        <f t="shared" ref="AF1" si="23">AE1+AE1-AD1</f>
+        <v>87</v>
       </c>
       <c r="AG1">
-        <f t="shared" ref="AG1" si="8">AF1+AF1-AE1</f>
-        <v>30</v>
+        <f t="shared" ref="AG1" si="24">AF1+AF1-AE1</f>
+        <v>90</v>
       </c>
       <c r="AH1">
-        <f t="shared" ref="AH1" si="9">AG1+AG1-AF1</f>
-        <v>31</v>
+        <f t="shared" ref="AH1" si="25">AG1+AG1-AF1</f>
+        <v>93</v>
       </c>
       <c r="AI1">
-        <f t="shared" ref="AI1" si="10">AH1+AH1-AG1</f>
-        <v>32</v>
+        <f t="shared" ref="AI1" si="26">AH1+AH1-AG1</f>
+        <v>96</v>
       </c>
       <c r="AJ1">
-        <f t="shared" ref="AJ1" si="11">AI1+AI1-AH1</f>
-        <v>33</v>
+        <f t="shared" ref="AJ1" si="27">AI1+AI1-AH1</f>
+        <v>99</v>
       </c>
       <c r="AK1">
-        <f t="shared" ref="AK1" si="12">AJ1+AJ1-AI1</f>
-        <v>34</v>
+        <f t="shared" ref="AK1" si="28">AJ1+AJ1-AI1</f>
+        <v>102</v>
+      </c>
+      <c r="AL1">
+        <f t="shared" ref="AL1" si="29">AK1+AK1-AJ1</f>
+        <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -653,13 +702,13 @@
         <v>0.1</v>
       </c>
       <c r="T2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="U2">
         <v>0.5</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="W2">
         <v>1</v>
@@ -671,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="Z2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AA2">
         <v>0.3</v>
@@ -706,11 +755,14 @@
       <c r="AK2">
         <v>0.3</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AL2">
+        <v>0.3</v>
+      </c>
+      <c r="AM2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -781,13 +833,13 @@
         <v>1</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -820,13 +872,16 @@
         <v>1</v>
       </c>
       <c r="AK3">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -855,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -897,7 +952,7 @@
         <v>0</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4">
         <v>1</v>
@@ -912,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="AC4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -936,13 +991,16 @@
         <v>0</v>
       </c>
       <c r="AK4">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -995,7 +1053,7 @@
         <v>3</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -1043,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="AH5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AI5">
         <v>3</v>
@@ -1054,11 +1112,14 @@
       <c r="AK5">
         <v>3</v>
       </c>
-      <c r="AL5" s="2" t="s">
+      <c r="AL5">
+        <v>3</v>
+      </c>
+      <c r="AM5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1172,7 @@
         <v>2</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -1159,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="AH6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI6">
         <v>2</v>
@@ -1170,11 +1231,14 @@
       <c r="AK6">
         <v>2</v>
       </c>
-      <c r="AL6" s="2" t="s">
+      <c r="AL6">
+        <v>2</v>
+      </c>
+      <c r="AM6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1200,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -1209,7 +1273,7 @@
         <v>2</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -1218,67 +1282,67 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <v>1</v>
       </c>
       <c r="V7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
         <v>2</v>
@@ -1286,13 +1350,16 @@
       <c r="AK7">
         <v>2</v>
       </c>
-      <c r="AL7" s="2" t="s">
+      <c r="AL7">
+        <v>2</v>
+      </c>
+      <c r="AM7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
@@ -1304,7 +1371,7 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1316,7 +1383,7 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <v>2</v>
@@ -1325,7 +1392,7 @@
         <v>2</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -1337,16 +1404,16 @@
         <v>1</v>
       </c>
       <c r="P8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <v>1</v>
@@ -1355,60 +1422,63 @@
         <v>1</v>
       </c>
       <c r="V8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK8">
-        <v>2</v>
-      </c>
-      <c r="AL8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>14</v>
@@ -1423,7 +1493,7 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1432,13 +1502,13 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>2</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1456,16 +1526,16 @@
         <v>1</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U9">
         <v>1</v>
@@ -1516,51 +1586,54 @@
         <v>1</v>
       </c>
       <c r="AK9">
-        <v>2</v>
-      </c>
-      <c r="AL9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AM9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -1602,10 +1675,10 @@
         <v>1</v>
       </c>
       <c r="AA10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC10">
         <v>1</v>
@@ -1614,10 +1687,10 @@
         <v>1</v>
       </c>
       <c r="AE10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10">
         <v>1</v>
@@ -1629,265 +1702,274 @@
         <v>1</v>
       </c>
       <c r="AJ10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK10">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL10">
+        <v>2</v>
+      </c>
+      <c r="AM10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N11">
-        <v>0.16</v>
+        <v>2</v>
       </c>
       <c r="O11">
-        <v>0.16</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <v>-0.16</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <v>-0.16</v>
+        <v>2</v>
       </c>
       <c r="R11">
-        <v>-0.16</v>
+        <v>2</v>
       </c>
       <c r="S11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="V11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W11">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="X11">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Y11">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="Z11">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AA11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AE11">
-        <v>0.16</v>
+        <v>2</v>
       </c>
       <c r="AF11">
-        <v>0.16</v>
+        <v>2</v>
       </c>
       <c r="AG11">
-        <v>0.16</v>
+        <v>2</v>
       </c>
       <c r="AH11">
-        <v>0.16</v>
+        <v>2</v>
       </c>
       <c r="AI11">
-        <v>0.16</v>
+        <v>2</v>
       </c>
       <c r="AJ11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK11">
-        <v>0</v>
-      </c>
-      <c r="AL11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL11">
+        <v>2</v>
+      </c>
+      <c r="AM11" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12">
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="T12">
-        <v>-0.2</v>
+        <v>1</v>
       </c>
       <c r="U12">
-        <v>-0.2</v>
+        <v>1</v>
       </c>
       <c r="V12">
-        <v>-0.2</v>
+        <v>1</v>
       </c>
       <c r="W12">
-        <v>-0.2</v>
+        <v>1</v>
       </c>
       <c r="X12">
-        <v>-0.2</v>
+        <v>1</v>
       </c>
       <c r="Y12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK12">
-        <v>0</v>
-      </c>
-      <c r="AL12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL12">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1899,13 +1981,13 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -1982,31 +2064,34 @@
       <c r="AK13">
         <v>1</v>
       </c>
-      <c r="AL13" s="2" t="s">
+      <c r="AL13">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2015,16 +2100,16 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -2093,57 +2178,60 @@
         <v>1</v>
       </c>
       <c r="AJ14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK14">
-        <v>1</v>
-      </c>
-      <c r="AL14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL14">
+        <v>2</v>
+      </c>
+      <c r="AM14" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -2152,16 +2240,16 @@
         <v>1</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U15">
         <v>1</v>
@@ -2170,13 +2258,13 @@
         <v>1</v>
       </c>
       <c r="W15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z15">
         <v>1</v>
@@ -2194,38 +2282,2715 @@
         <v>1</v>
       </c>
       <c r="AE15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK15">
-        <v>1</v>
-      </c>
-      <c r="AL15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL15">
+        <v>2</v>
+      </c>
+      <c r="AM15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="18:18" x14ac:dyDescent="0.3">
-      <c r="R19" t="s">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>1</v>
+      </c>
+      <c r="AE16">
+        <v>1</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <v>1</v>
+      </c>
+      <c r="AI16">
+        <v>1</v>
+      </c>
+      <c r="AJ16">
+        <v>1</v>
+      </c>
+      <c r="AK16">
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0.16</v>
+      </c>
+      <c r="P17">
+        <v>0.08</v>
+      </c>
+      <c r="Q17">
+        <v>-0.08</v>
+      </c>
+      <c r="R17">
+        <v>-0.1</v>
+      </c>
+      <c r="S17">
+        <v>-0.16</v>
+      </c>
+      <c r="T17">
+        <v>-0.2</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>-1</v>
+      </c>
+      <c r="X17">
+        <v>-1</v>
+      </c>
+      <c r="Y17">
+        <v>-1</v>
+      </c>
+      <c r="Z17">
+        <v>0.2</v>
+      </c>
+      <c r="AA17">
+        <v>0.2</v>
+      </c>
+      <c r="AB17">
+        <v>-1</v>
+      </c>
+      <c r="AC17">
+        <v>-1</v>
+      </c>
+      <c r="AD17">
+        <v>-1</v>
+      </c>
+      <c r="AE17">
+        <v>-1</v>
+      </c>
+      <c r="AF17">
+        <v>0.16</v>
+      </c>
+      <c r="AG17">
+        <v>0.16</v>
+      </c>
+      <c r="AH17">
+        <v>0.1</v>
+      </c>
+      <c r="AI17">
+        <v>0.2</v>
+      </c>
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0.1</v>
+      </c>
+      <c r="P18">
+        <v>0.1</v>
+      </c>
+      <c r="Q18">
+        <v>0.05</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0.2</v>
+      </c>
+      <c r="U18">
+        <v>-0.2</v>
+      </c>
+      <c r="V18">
+        <v>-0.2</v>
+      </c>
+      <c r="W18">
+        <v>-0.2</v>
+      </c>
+      <c r="X18">
+        <v>-0.2</v>
+      </c>
+      <c r="Y18">
+        <v>-0.2</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>0.05</v>
+      </c>
+      <c r="AI18">
+        <v>0.1</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>1</v>
+      </c>
+      <c r="AD19">
+        <v>1</v>
+      </c>
+      <c r="AE19">
+        <v>1</v>
+      </c>
+      <c r="AF19">
+        <v>1</v>
+      </c>
+      <c r="AG19">
+        <v>1</v>
+      </c>
+      <c r="AH19">
+        <v>1</v>
+      </c>
+      <c r="AI19">
+        <v>1</v>
+      </c>
+      <c r="AJ19">
+        <v>1</v>
+      </c>
+      <c r="AK19">
+        <v>1</v>
+      </c>
+      <c r="AL19">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+      <c r="AD20">
+        <v>1</v>
+      </c>
+      <c r="AE20">
+        <v>1</v>
+      </c>
+      <c r="AF20">
+        <v>1</v>
+      </c>
+      <c r="AG20">
+        <v>1</v>
+      </c>
+      <c r="AH20">
+        <v>1</v>
+      </c>
+      <c r="AI20">
+        <v>1</v>
+      </c>
+      <c r="AJ20">
+        <v>1</v>
+      </c>
+      <c r="AK20">
+        <v>1</v>
+      </c>
+      <c r="AL20">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
+        <v>1</v>
+      </c>
+      <c r="AC21">
+        <v>1</v>
+      </c>
+      <c r="AD21">
+        <v>1</v>
+      </c>
+      <c r="AE21">
+        <v>1</v>
+      </c>
+      <c r="AF21">
+        <v>1</v>
+      </c>
+      <c r="AG21">
+        <v>1</v>
+      </c>
+      <c r="AH21">
+        <v>1</v>
+      </c>
+      <c r="AI21">
+        <v>1</v>
+      </c>
+      <c r="AJ21">
+        <v>1</v>
+      </c>
+      <c r="AK21">
+        <v>1</v>
+      </c>
+      <c r="AL21">
+        <v>1</v>
+      </c>
+      <c r="AM21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>1</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AB22">
+        <v>1</v>
+      </c>
+      <c r="AC22">
+        <v>1</v>
+      </c>
+      <c r="AD22">
+        <v>1</v>
+      </c>
+      <c r="AE22">
+        <v>1</v>
+      </c>
+      <c r="AF22">
+        <v>1</v>
+      </c>
+      <c r="AG22">
+        <v>1</v>
+      </c>
+      <c r="AH22">
+        <v>1</v>
+      </c>
+      <c r="AI22">
+        <v>1</v>
+      </c>
+      <c r="AJ22">
+        <v>1</v>
+      </c>
+      <c r="AK22">
+        <v>1</v>
+      </c>
+      <c r="AL22">
+        <v>1</v>
+      </c>
+      <c r="AM22" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.05</v>
+      </c>
+      <c r="E23">
+        <v>0.3</v>
+      </c>
+      <c r="F23">
+        <v>0.7</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0.5</v>
+      </c>
+      <c r="I23">
+        <v>0.7</v>
+      </c>
+      <c r="J23">
+        <v>0.7</v>
+      </c>
+      <c r="K23">
+        <v>0.3</v>
+      </c>
+      <c r="L23">
+        <v>0.1</v>
+      </c>
+      <c r="M23">
+        <v>0.2</v>
+      </c>
+      <c r="N23">
+        <v>0.3</v>
+      </c>
+      <c r="O23">
+        <v>0.1</v>
+      </c>
+      <c r="P23">
+        <v>0.1</v>
+      </c>
+      <c r="Q23">
+        <v>0.3</v>
+      </c>
+      <c r="R23">
+        <v>0.4</v>
+      </c>
+      <c r="S23">
+        <v>0.7</v>
+      </c>
+      <c r="T23">
+        <v>0.8</v>
+      </c>
+      <c r="U23">
+        <v>0.9</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
+        <v>1</v>
+      </c>
+      <c r="Y23">
+        <v>0.7</v>
+      </c>
+      <c r="Z23">
+        <v>0.4</v>
+      </c>
+      <c r="AA23">
+        <v>0.3</v>
+      </c>
+      <c r="AB23">
+        <v>0.1</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0.3</v>
+      </c>
+      <c r="AF23">
+        <v>0.6</v>
+      </c>
+      <c r="AG23">
+        <v>0.1</v>
+      </c>
+      <c r="AH23">
+        <v>0.2</v>
+      </c>
+      <c r="AI23">
+        <v>0.1</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="S25" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <f>IF(C6=2,0,"GF")</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:AL26" si="30">IF(D6=2,0,"GF")</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="S26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="T26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="U26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="V26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="W26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="X26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="Y26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="Z26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="AA26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="AB26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="AC26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="AD26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="AE26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="AF26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="AG26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="AH26" t="str">
+        <f t="shared" si="30"/>
+        <v>GF</v>
+      </c>
+      <c r="AI26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="AJ26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="AK26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="AL26">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <f>IF(OR(C3=0,C4=1),0,IF(C5=3,"GF",C2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>IF(OR(D3=0,D4=1),0,IF(D5=3,"GF",D2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>IF(OR(E3=0,E4=1),0,IF(E5=3,"GF",E2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>IF(OR(F3=0,F4=1),0,IF(F5=3,"GF",F2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>IF(OR(G3=0,G4=1),0,IF(G5=3,"GF",G2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f>IF(OR(H3=0,H4=1),0,IF(H5=3,"GF",H2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f>IF(OR(I3=0,I4=1),0,IF(I5=3,"GF",I2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f>IF(OR(J3=0,J4=1),0,IF(J5=3,"GF",J2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="K27" t="str">
+        <f>IF(OR(K3=0,K4=1),0,IF(K5=3,"GF",K2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="L27" t="str">
+        <f>IF(OR(L3=0,L4=1),0,IF(L5=3,"GF",L2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="M27" t="str">
+        <f>IF(OR(M3=0,M4=1),0,IF(M5=3,"GF",M2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="N27" t="str">
+        <f>IF(OR(N3=0,N4=1),0,IF(N5=3,"GF",N2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="O27" t="str">
+        <f>IF(OR(O3=0,O4=1),0,IF(O5=3,"GF",O2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="P27" t="str">
+        <f>IF(OR(P3=0,P4=1),0,IF(P5=3,"GF",P2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="Q27" t="str">
+        <f>IF(OR(Q3=0,Q4=1),0,IF(Q5=3,"GF",Q2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="R27" t="str">
+        <f>IF(OR(R3=0,R4=1),0,IF(R5=3,"GF",R2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="S27">
+        <f>IF(OR(S3=0,S4=1),0,IF(S5=3,"GF",S2*0.9*80))</f>
+        <v>7.2000000000000011</v>
+      </c>
+      <c r="T27">
+        <f>IF(OR(T3=0,T4=1),0,IF(T5=3,"GF",T2*0.9*80))</f>
+        <v>7.2000000000000011</v>
+      </c>
+      <c r="U27">
+        <f>IF(OR(U3=0,U4=1),0,IF(U5=3,"GF",U2*0.9*80))</f>
+        <v>36</v>
+      </c>
+      <c r="V27">
+        <f>IF(OR(V3=0,V4=1),0,IF(V5=3,"GF",V2*0.9*80))</f>
+        <v>36</v>
+      </c>
+      <c r="W27">
+        <f>IF(OR(W3=0,W4=1),0,IF(W5=3,"GF",W2*0.9*80))</f>
+        <v>72</v>
+      </c>
+      <c r="X27">
+        <f>IF(OR(X3=0,X4=1),0,IF(X5=3,"GF",X2*0.9*80))</f>
+        <v>72</v>
+      </c>
+      <c r="Y27">
+        <f>IF(OR(Y3=0,Y4=1),0,IF(Y5=3,"GF",Y2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <f>IF(OR(Z3=0,Z4=1),0,IF(Z5=3,"GF",Z2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <f>IF(OR(AA3=0,AA4=1),0,IF(AA5=3,"GF",AA2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <f>IF(OR(AB3=0,AB4=1),0,IF(AB5=3,"GF",AB2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <f>IF(OR(AC3=0,AC4=1),0,IF(AC5=3,"GF",AC2*0.9*80))</f>
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <f>IF(OR(AD3=0,AD4=1),0,IF(AD5=3,"GF",AD2*0.9*80))</f>
+        <v>21.6</v>
+      </c>
+      <c r="AE27">
+        <f>IF(OR(AE3=0,AE4=1),0,IF(AE5=3,"GF",AE2*0.9*80))</f>
+        <v>21.6</v>
+      </c>
+      <c r="AF27">
+        <f>IF(OR(AF3=0,AF4=1),0,IF(AF5=3,"GF",AF2*0.9*80))</f>
+        <v>21.6</v>
+      </c>
+      <c r="AG27">
+        <f>IF(OR(AG3=0,AG4=1),0,IF(AG5=3,"GF",AG2*0.9*80))</f>
+        <v>21.6</v>
+      </c>
+      <c r="AH27">
+        <f>IF(OR(AH3=0,AH4=1),0,IF(AH5=3,"GF",AH2*0.9*80))</f>
+        <v>21.6</v>
+      </c>
+      <c r="AI27" t="str">
+        <f>IF(OR(AI3=0,AI4=1),0,IF(AI5=3,"GF",AI2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="AJ27" t="str">
+        <f>IF(OR(AJ3=0,AJ4=1),0,IF(AJ5=3,"GF",AJ2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="AK27" t="str">
+        <f>IF(OR(AK3=0,AK4=1),0,IF(AK5=3,"GF",AK2*0.9*80))</f>
+        <v>GF</v>
+      </c>
+      <c r="AL27">
+        <f>IF(OR(AL3=0,AL4=1),0,IF(AL5=3,"GF",AL2*0.9*80))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <f>IF(OR(C16=0,C16=0),0,IF(C21=0,"GF",C17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="D28" t="str">
+        <f>IF(OR(D16=0,D16=0),0,IF(D21=0,"GF",D17*250))</f>
+        <v>GF</v>
+      </c>
+      <c r="E28" t="str">
+        <f>IF(OR(E16=0,E16=0),0,IF(E21=0,"GF",E17*250))</f>
+        <v>GF</v>
+      </c>
+      <c r="F28" t="str">
+        <f>IF(OR(F16=0,F16=0),0,IF(F21=0,"GF",F17*250))</f>
+        <v>GF</v>
+      </c>
+      <c r="G28" t="str">
+        <f>IF(OR(G16=0,G16=0),0,IF(G21=0,"GF",G17*250))</f>
+        <v>GF</v>
+      </c>
+      <c r="H28" t="str">
+        <f>IF(OR(H16=0,H16=0),0,IF(H21=0,"GF",H17*250))</f>
+        <v>GF</v>
+      </c>
+      <c r="I28" t="str">
+        <f>IF(OR(I16=0,I16=0),0,IF(I21=0,"GF",I17*250))</f>
+        <v>GF</v>
+      </c>
+      <c r="J28">
+        <f>IF(OR(J16=0,J16=0),0,IF(J21=0,"GF",J17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>IF(OR(K16=0,K16=0),0,IF(K21=0,"GF",K17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>IF(OR(L16=0,L16=0),0,IF(L21=0,"GF",L17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f>IF(OR(M16=0,M16=0),0,IF(M21=0,"GF",M17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f>IF(OR(N16=0,N16=0),0,IF(N21=0,"GF",N17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f>IF(OR(O16=0,O16=0),0,IF(O21=0,"GF",O17*250))</f>
+        <v>40</v>
+      </c>
+      <c r="P28">
+        <f>IF(OR(P16=0,P16=0),0,IF(P21=0,"GF",P17*250))</f>
+        <v>20</v>
+      </c>
+      <c r="Q28">
+        <f>IF(OR(Q16=0,Q16=0),0,IF(Q21=0,"GF",Q17*250))</f>
+        <v>-20</v>
+      </c>
+      <c r="R28">
+        <f>IF(OR(R16=0,R16=0),0,IF(R21=0,"GF",R17*250))</f>
+        <v>-25</v>
+      </c>
+      <c r="S28">
+        <f>IF(OR(S16=0,S16=0),0,IF(S21=0,"GF",S17*250))</f>
+        <v>-40</v>
+      </c>
+      <c r="T28">
+        <f>IF(OR(T16=0,T16=0),0,IF(T21=0,"GF",T17*250))</f>
+        <v>-50</v>
+      </c>
+      <c r="U28">
+        <f>IF(OR(U16=0,U16=0),0,IF(U21=0,"GF",U17*250))</f>
+        <v>250</v>
+      </c>
+      <c r="V28">
+        <f>IF(OR(V16=0,V16=0),0,IF(V21=0,"GF",V17*250))</f>
+        <v>250</v>
+      </c>
+      <c r="W28">
+        <f>IF(OR(W16=0,W16=0),0,IF(W21=0,"GF",W17*250))</f>
+        <v>-250</v>
+      </c>
+      <c r="X28">
+        <f>IF(OR(X16=0,X16=0),0,IF(X21=0,"GF",X17*250))</f>
+        <v>-250</v>
+      </c>
+      <c r="Y28">
+        <f>IF(OR(Y16=0,Y16=0),0,IF(Y21=0,"GF",Y17*250))</f>
+        <v>-250</v>
+      </c>
+      <c r="Z28">
+        <f>IF(OR(Z16=0,Z16=0),0,IF(Z21=0,"GF",Z17*250))</f>
+        <v>50</v>
+      </c>
+      <c r="AA28">
+        <f>IF(OR(AA16=0,AA16=0),0,IF(AA21=0,"GF",AA17*250))</f>
+        <v>50</v>
+      </c>
+      <c r="AB28">
+        <f>IF(OR(AB16=0,AB16=0),0,IF(AB21=0,"GF",AB17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="AC28">
+        <f>IF(OR(AC16=0,AC16=0),0,IF(AC21=0,"GF",AC17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="AD28">
+        <f>IF(OR(AD16=0,AD16=0),0,IF(AD21=0,"GF",AD17*250))</f>
+        <v>-250</v>
+      </c>
+      <c r="AE28">
+        <f>IF(OR(AE16=0,AE16=0),0,IF(AE21=0,"GF",AE17*250))</f>
+        <v>-250</v>
+      </c>
+      <c r="AF28">
+        <f>IF(OR(AF16=0,AF16=0),0,IF(AF21=0,"GF",AF17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="AG28">
+        <f>IF(OR(AG16=0,AG16=0),0,IF(AG21=0,"GF",AG17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="AH28">
+        <f>IF(OR(AH16=0,AH16=0),0,IF(AH21=0,"GF",AH17*250))</f>
+        <v>25</v>
+      </c>
+      <c r="AI28">
+        <f>IF(OR(AI16=0,AI16=0),0,IF(AI21=0,"GF",AI17*250))</f>
+        <v>50</v>
+      </c>
+      <c r="AJ28">
+        <f>IF(OR(AJ16=0,AJ16=0),0,IF(AJ21=0,"GF",AJ17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="AK28">
+        <f>IF(OR(AK16=0,AK16=0),0,IF(AK21=0,"GF",AK17*250))</f>
+        <v>0</v>
+      </c>
+      <c r="AL28">
+        <f>IF(OR(AL16=0,AL16=0),0,IF(AL21=0,"GF",AL17*250))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <f>IF(C22=0,0,C23*100)</f>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f>IF(D22=0,0,D23*100)</f>
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <f>IF(E22=0,0,E23*100)</f>
+        <v>30</v>
+      </c>
+      <c r="F29">
+        <f>IF(F22=0,0,F23*100)</f>
+        <v>70</v>
+      </c>
+      <c r="G29">
+        <f>IF(G22=0,0,G23*100)</f>
+        <v>100</v>
+      </c>
+      <c r="H29">
+        <f>IF(H22=0,0,H23*100)</f>
+        <v>50</v>
+      </c>
+      <c r="I29">
+        <f>IF(I22=0,0,I23*100)</f>
+        <v>70</v>
+      </c>
+      <c r="J29">
+        <f>IF(J22=0,0,J23*100)</f>
+        <v>70</v>
+      </c>
+      <c r="K29">
+        <f>IF(K22=0,0,K23*100)</f>
+        <v>30</v>
+      </c>
+      <c r="L29">
+        <f>IF(L22=0,0,L23*100)</f>
+        <v>10</v>
+      </c>
+      <c r="M29">
+        <f>IF(M22=0,0,M23*100)</f>
+        <v>20</v>
+      </c>
+      <c r="N29">
+        <f>IF(N22=0,0,N23*100)</f>
+        <v>30</v>
+      </c>
+      <c r="O29">
+        <f>IF(O22=0,0,O23*100)</f>
+        <v>10</v>
+      </c>
+      <c r="P29">
+        <f>IF(P22=0,0,P23*100)</f>
+        <v>10</v>
+      </c>
+      <c r="Q29">
+        <f>IF(Q22=0,0,Q23*100)</f>
+        <v>30</v>
+      </c>
+      <c r="R29">
+        <f>IF(R22=0,0,R23*100)</f>
+        <v>40</v>
+      </c>
+      <c r="S29">
+        <f>IF(S22=0,0,S23*100)</f>
+        <v>70</v>
+      </c>
+      <c r="T29">
+        <f>IF(T22=0,0,T23*100)</f>
+        <v>80</v>
+      </c>
+      <c r="U29">
+        <f>IF(U22=0,0,U23*100)</f>
+        <v>90</v>
+      </c>
+      <c r="V29">
+        <f>IF(V22=0,0,V23*100)</f>
+        <v>100</v>
+      </c>
+      <c r="W29">
+        <f>IF(W22=0,0,W23*100)</f>
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <f>IF(X22=0,0,X23*100)</f>
+        <v>100</v>
+      </c>
+      <c r="Y29">
+        <f>IF(Y22=0,0,Y23*100)</f>
+        <v>70</v>
+      </c>
+      <c r="Z29">
+        <f>IF(Z22=0,0,Z23*100)</f>
+        <v>40</v>
+      </c>
+      <c r="AA29">
+        <f>IF(AA22=0,0,AA23*100)</f>
+        <v>30</v>
+      </c>
+      <c r="AB29">
+        <f>IF(AB22=0,0,AB23*100)</f>
+        <v>10</v>
+      </c>
+      <c r="AC29">
+        <f>IF(AC22=0,0,AC23*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD29">
+        <f>IF(AD22=0,0,AD23*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AE29">
+        <f>IF(AE22=0,0,AE23*100)</f>
+        <v>30</v>
+      </c>
+      <c r="AF29">
+        <f>IF(AF22=0,0,AF23*100)</f>
+        <v>60</v>
+      </c>
+      <c r="AG29">
+        <f>IF(AG22=0,0,AG23*100)</f>
+        <v>10</v>
+      </c>
+      <c r="AH29">
+        <f>IF(AH22=0,0,AH23*100)</f>
+        <v>20</v>
+      </c>
+      <c r="AI29">
+        <f>IF(AI22=0,0,AI23*100)</f>
+        <v>10</v>
+      </c>
+      <c r="AJ29">
+        <f>IF(AJ22=0,0,AJ23*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AK29">
+        <f>IF(AK22=0,0,AK23*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AL29">
+        <f>IF(AL22=0,0,AL23*100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <f>(IF(C8=2,0,3)+IF(C9=2,0,25)+IF(C10=2,0,10)+IF(C11=2,0,15)+IF(C13=2,0,20)+IF(C14=2,0,10)+IF(C15=2,0,20))*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30:AL30" si="31">(IF(D8=2,0,3)+IF(D9=2,0,25)+IF(D10=2,0,10)+IF(D11=2,0,15)+IF(D13=2,0,20)+IF(D14=2,0,10)+IF(D15=2,0,20))*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="31"/>
+        <v>2.7</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="31"/>
+        <v>25.2</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="31"/>
+        <v>43.2</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="31"/>
+        <v>61.2</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="31"/>
+        <v>92.7</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="31"/>
+        <v>22.5</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="31"/>
+        <v>43.2</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="31"/>
+        <v>61.2</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="31"/>
+        <v>92.7</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="31"/>
+        <v>92.7</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="31"/>
+        <v>38.700000000000003</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="31"/>
+        <v>38.700000000000003</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="31"/>
+        <v>38.700000000000003</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="31"/>
+        <v>38.700000000000003</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="31"/>
+        <v>92.7</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="31"/>
+        <v>92.7</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="31"/>
+        <v>61.2</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="31"/>
+        <v>61.2</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="31"/>
+        <v>74.7</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="31"/>
+        <v>92.7</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="31"/>
+        <v>92.7</v>
+      </c>
+      <c r="AB30">
+        <f t="shared" si="31"/>
+        <v>92.7</v>
+      </c>
+      <c r="AC30">
+        <f t="shared" si="31"/>
+        <v>92.7</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="31"/>
+        <v>92.7</v>
+      </c>
+      <c r="AE30">
+        <f t="shared" si="31"/>
+        <v>61.2</v>
+      </c>
+      <c r="AF30">
+        <f t="shared" si="31"/>
+        <v>61.2</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="31"/>
+        <v>61.2</v>
+      </c>
+      <c r="AH30">
+        <f t="shared" si="31"/>
+        <v>61.2</v>
+      </c>
+      <c r="AI30">
+        <f t="shared" si="31"/>
+        <v>61.2</v>
+      </c>
+      <c r="AJ30">
+        <f t="shared" si="31"/>
+        <v>43.2</v>
+      </c>
+      <c r="AK30">
+        <f t="shared" si="31"/>
+        <v>43.2</v>
+      </c>
+      <c r="AL30">
+        <f t="shared" si="31"/>
+        <v>43.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <f>-SUM(C26:C29)+C30</f>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f>-SUM(D26:D29)+D30</f>
+        <v>-5</v>
+      </c>
+      <c r="E32">
+        <f>-SUM(E26:E29)+E30</f>
+        <v>-27.3</v>
+      </c>
+      <c r="F32">
+        <f>-SUM(F26:F29)+F30</f>
+        <v>-44.8</v>
+      </c>
+      <c r="G32">
+        <f>-SUM(G26:G29)+G30</f>
+        <v>-56.8</v>
+      </c>
+      <c r="H32">
+        <f>-SUM(H26:H29)+H30</f>
+        <v>11.200000000000003</v>
+      </c>
+      <c r="I32">
+        <f>-SUM(I26:I29)+I30</f>
+        <v>22.700000000000003</v>
+      </c>
+      <c r="J32">
+        <f>-SUM(J26:J29)+J30</f>
+        <v>-70</v>
+      </c>
+      <c r="K32">
+        <f>-SUM(K26:K29)+K30</f>
+        <v>-30</v>
+      </c>
+      <c r="L32">
+        <f>-SUM(L26:L29)+L30</f>
+        <v>12.5</v>
+      </c>
+      <c r="M32">
+        <f>-SUM(M26:M29)+M30</f>
+        <v>23.200000000000003</v>
+      </c>
+      <c r="N32">
+        <f>-SUM(N26:N29)+N30</f>
+        <v>31.200000000000003</v>
+      </c>
+      <c r="O32">
+        <f>-SUM(O26:O29)+O30</f>
+        <v>42.7</v>
+      </c>
+      <c r="P32">
+        <f>-SUM(P26:P29)+P30</f>
+        <v>62.7</v>
+      </c>
+      <c r="Q32">
+        <f>-SUM(Q26:Q29)+Q30</f>
+        <v>28.700000000000003</v>
+      </c>
+      <c r="R32">
+        <f>-SUM(R26:R29)+R30</f>
+        <v>23.700000000000003</v>
+      </c>
+      <c r="S32">
+        <f>-SUM(S26:S29)+S30</f>
+        <v>1.5</v>
+      </c>
+      <c r="T32">
+        <f>-SUM(T26:T29)+T30</f>
+        <v>1.5</v>
+      </c>
+      <c r="U32">
+        <f>-SUM(U26:U29)+U30</f>
+        <v>-283.3</v>
+      </c>
+      <c r="V32">
+        <f>-SUM(V26:V29)+V30</f>
+        <v>-293.3</v>
+      </c>
+      <c r="W32">
+        <f>-SUM(W26:W29)+W30</f>
+        <v>239.2</v>
+      </c>
+      <c r="X32">
+        <f>-SUM(X26:X29)+X30</f>
+        <v>139.19999999999999</v>
+      </c>
+      <c r="Y32">
+        <f>-SUM(Y26:Y29)+Y30</f>
+        <v>254.7</v>
+      </c>
+      <c r="Z32">
+        <f>-SUM(Z26:Z29)+Z30</f>
+        <v>2.7000000000000028</v>
+      </c>
+      <c r="AA32">
+        <f>-SUM(AA26:AA29)+AA30</f>
+        <v>12.700000000000003</v>
+      </c>
+      <c r="AB32">
+        <f>-SUM(AB26:AB29)+AB30</f>
+        <v>82.7</v>
+      </c>
+      <c r="AC32">
+        <f>-SUM(AC26:AC29)+AC30</f>
+        <v>92.7</v>
+      </c>
+      <c r="AD32">
+        <f>-SUM(AD26:AD29)+AD30</f>
+        <v>321.10000000000002</v>
+      </c>
+      <c r="AE32">
+        <f>-SUM(AE26:AE29)+AE30</f>
+        <v>259.60000000000002</v>
+      </c>
+      <c r="AF32">
+        <f>-SUM(AF26:AF29)+AF30</f>
+        <v>-20.399999999999991</v>
+      </c>
+      <c r="AG32">
+        <f>-SUM(AG26:AG29)+AG30</f>
+        <v>29.6</v>
+      </c>
+      <c r="AH32">
+        <f>-SUM(AH26:AH29)+AH30</f>
+        <v>-5.3999999999999915</v>
+      </c>
+      <c r="AI32">
+        <f>-SUM(AI26:AI29)+AI30</f>
+        <v>1.2000000000000028</v>
+      </c>
+      <c r="AJ32">
+        <f>-SUM(AJ26:AJ29)+AJ30</f>
+        <v>43.2</v>
+      </c>
+      <c r="AK32">
+        <f>-SUM(AK26:AK29)+AK30</f>
+        <v>43.2</v>
+      </c>
+      <c r="AL32">
+        <f>-SUM(AL26:AL29)+AL30</f>
+        <v>43.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34">
+        <f>IF(OR(C3=0,C4=1),0,IF(C5=3,"GF",C2*0.43*80))</f>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ref="D34:AL34" si="32">IF(OR(D3=0,D4=1),0,IF(D5=3,"GF",D2*0.43*80))</f>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="R34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="32"/>
+        <v>3.4400000000000004</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="32"/>
+        <v>3.4400000000000004</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="32"/>
+        <v>17.2</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="32"/>
+        <v>17.2</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="32"/>
+        <v>34.4</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="32"/>
+        <v>34.4</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AC34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AD34">
+        <f t="shared" si="32"/>
+        <v>10.32</v>
+      </c>
+      <c r="AE34">
+        <f t="shared" si="32"/>
+        <v>10.32</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="32"/>
+        <v>10.32</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="32"/>
+        <v>10.32</v>
+      </c>
+      <c r="AH34">
+        <f t="shared" si="32"/>
+        <v>10.32</v>
+      </c>
+      <c r="AI34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="AJ34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="AK34" t="str">
+        <f t="shared" si="32"/>
+        <v>GF</v>
+      </c>
+      <c r="AL34">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <f>IF(OR(C16=0,C16=0),0,IF(C21=0,"GF",C18*250))</f>
+        <v>0</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" ref="D35:AL35" si="33">IF(OR(D16=0,D16=0),0,IF(D21=0,"GF",D18*250))</f>
+        <v>GF</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="33"/>
+        <v>GF</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="33"/>
+        <v>GF</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="33"/>
+        <v>GF</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="33"/>
+        <v>GF</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="33"/>
+        <v>GF</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="33"/>
+        <v>25</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="33"/>
+        <v>25</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="33"/>
+        <v>12.5</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="33"/>
+        <v>50</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="33"/>
+        <v>-50</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="33"/>
+        <v>-50</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="33"/>
+        <v>-50</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="33"/>
+        <v>-50</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="33"/>
+        <v>-50</v>
+      </c>
+      <c r="Z35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AB35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AC35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AD35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AE35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AF35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AH35">
+        <f t="shared" si="33"/>
+        <v>12.5</v>
+      </c>
+      <c r="AI35">
+        <f t="shared" si="33"/>
+        <v>25</v>
+      </c>
+      <c r="AJ35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AK35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AL35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36">
+        <f>IF(C30=0,0,C31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <f>IF(D30=0,0,D31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <f>IF(E30=0,0,E31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f>IF(F30=0,0,F31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f>IF(G30=0,0,G31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <f>IF(H30=0,0,H31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f>IF(I30=0,0,I31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f>IF(J30=0,0,J31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f>IF(K30=0,0,K31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f>IF(L30=0,0,L31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f>IF(M30=0,0,M31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <f>IF(N30=0,0,N31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f>IF(O30=0,0,O31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <f>IF(P30=0,0,P31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <f>IF(Q30=0,0,Q31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <f>IF(R30=0,0,R31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <f>IF(S30=0,0,S31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <f>IF(T30=0,0,T31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <f>IF(U30=0,0,U31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <f>IF(V30=0,0,V31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <f>IF(W30=0,0,W31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <f>IF(X30=0,0,X31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <f>IF(Y30=0,0,Y31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <f>IF(Z30=0,0,Z31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <f>IF(AA30=0,0,AA31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AB36">
+        <f>IF(AB30=0,0,AB31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <f>IF(AC30=0,0,AC31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <f>IF(AD30=0,0,AD31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <f>IF(AE30=0,0,AE31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <f>IF(AF30=0,0,AF31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AG36">
+        <f>IF(AG30=0,0,AG31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AH36">
+        <f>IF(AH30=0,0,AH31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AI36">
+        <f>IF(AI30=0,0,AI31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ36">
+        <f>IF(AJ30=0,0,AJ31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AK36">
+        <f>IF(AK30=0,0,AK31*100)</f>
+        <v>0</v>
+      </c>
+      <c r="AL36">
+        <f>IF(AL30=0,0,AL31*100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37">
+        <f>(IF(C8=2,0,3)+IF(C9=2,0,25)+IF(C10=2,0,10)+IF(C11=2,0,15)+IF(C13=2,0,20)+IF(C14=2,0,10)+IF(C15=2,0,20))*(SQRT(1-(0.9*0.9)))</f>
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ref="D37:AL37" si="34">(IF(D8=2,0,3)+IF(D9=2,0,25)+IF(D10=2,0,10)+IF(D11=2,0,15)+IF(D13=2,0,20)+IF(D14=2,0,10)+IF(D15=2,0,20))*(SQRT(1-(0.9*0.9)))</f>
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="34"/>
+        <v>1.3076696830622019</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="34"/>
+        <v>12.204917041913884</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="34"/>
+        <v>20.92271492899523</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="34"/>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="34"/>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="34"/>
+        <v>10.897247358851683</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="34"/>
+        <v>20.92271492899523</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="34"/>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="34"/>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="34"/>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="34"/>
+        <v>18.743265457224894</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="34"/>
+        <v>18.743265457224894</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="34"/>
+        <v>18.743265457224894</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="34"/>
+        <v>18.743265457224894</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="34"/>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="34"/>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="34"/>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="34"/>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="34"/>
+        <v>36.178861231387586</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" si="34"/>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" si="34"/>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" si="34"/>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="AC37">
+        <f t="shared" si="34"/>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="34"/>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="AE37">
+        <f t="shared" si="34"/>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="34"/>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="AG37">
+        <f t="shared" si="34"/>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="AH37">
+        <f t="shared" si="34"/>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="AI37">
+        <f t="shared" si="34"/>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="AJ37">
+        <f t="shared" si="34"/>
+        <v>20.92271492899523</v>
+      </c>
+      <c r="AK37">
+        <f t="shared" si="34"/>
+        <v>20.92271492899523</v>
+      </c>
+      <c r="AL37">
+        <f t="shared" si="34"/>
+        <v>20.92271492899523</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39">
+        <f>(IF(C8=2,0,3)+IF(C9=2,0,25)+IF(C10=2,0,10)+IF(C11=2,0,15)+IF(C13=2,0,20)+IF(C14=2,0,10)+IF(C15=2,0,20))*(SQRT(1-(0.9*0.9)))</f>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f>-SUM(D34:D36)+D37</f>
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <f>-SUM(E34:E36)+E37</f>
+        <v>1.3076696830622019</v>
+      </c>
+      <c r="F39">
+        <f>-SUM(F34:F36)+F37</f>
+        <v>12.204917041913884</v>
+      </c>
+      <c r="G39">
+        <f>-SUM(G34:G36)+G37</f>
+        <v>20.92271492899523</v>
+      </c>
+      <c r="H39">
+        <f>-SUM(H34:H36)+H37</f>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="I39">
+        <f>-SUM(I34:I36)+I37</f>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="J39">
+        <f>-SUM(J34:J36)+J37</f>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f>-SUM(K34:K36)+K37</f>
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <f>-SUM(L34:L36)+L37</f>
+        <v>10.897247358851683</v>
+      </c>
+      <c r="M39">
+        <f>-SUM(M34:M36)+M37</f>
+        <v>20.92271492899523</v>
+      </c>
+      <c r="N39">
+        <f>-SUM(N34:N36)+N37</f>
+        <v>29.640512816076576</v>
+      </c>
+      <c r="O39">
+        <f>-SUM(O34:O36)+O37</f>
+        <v>19.896659118468932</v>
+      </c>
+      <c r="P39">
+        <f>-SUM(P34:P36)+P37</f>
+        <v>19.896659118468932</v>
+      </c>
+      <c r="Q39">
+        <f>-SUM(Q34:Q36)+Q37</f>
+        <v>6.2432654572248936</v>
+      </c>
+      <c r="R39">
+        <f>-SUM(R34:R36)+R37</f>
+        <v>18.743265457224894</v>
+      </c>
+      <c r="S39">
+        <f>-SUM(S34:S36)+S37</f>
+        <v>15.303265457224892</v>
+      </c>
+      <c r="T39">
+        <f>-SUM(T34:T36)+T37</f>
+        <v>-34.696734542775104</v>
+      </c>
+      <c r="U39">
+        <f>-SUM(U34:U36)+U37</f>
+        <v>77.696659118468929</v>
+      </c>
+      <c r="V39">
+        <f>-SUM(V34:V36)+V37</f>
+        <v>77.696659118468929</v>
+      </c>
+      <c r="W39">
+        <f>-SUM(W34:W36)+W37</f>
+        <v>45.240512816076574</v>
+      </c>
+      <c r="X39">
+        <f>-SUM(X34:X36)+X37</f>
+        <v>45.240512816076574</v>
+      </c>
+      <c r="Y39">
+        <f>-SUM(Y34:Y36)+Y37</f>
+        <v>86.178861231387586</v>
+      </c>
+      <c r="Z39">
+        <f>-SUM(Z34:Z36)+Z37</f>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="AA39">
+        <f>-SUM(AA34:AA36)+AA37</f>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="AB39">
+        <f>-SUM(AB34:AB36)+AB37</f>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="AC39">
+        <f>-SUM(AC34:AC36)+AC37</f>
+        <v>44.896659118468932</v>
+      </c>
+      <c r="AD39">
+        <f>-SUM(AD34:AD36)+AD37</f>
+        <v>34.576659118468932</v>
+      </c>
+      <c r="AE39">
+        <f>-SUM(AE34:AE36)+AE37</f>
+        <v>19.320512816076576</v>
+      </c>
+      <c r="AF39">
+        <f>-SUM(AF34:AF36)+AF37</f>
+        <v>19.320512816076576</v>
+      </c>
+      <c r="AG39">
+        <f>-SUM(AG34:AG36)+AG37</f>
+        <v>19.320512816076576</v>
+      </c>
+      <c r="AH39">
+        <f>-SUM(AH34:AH36)+AH37</f>
+        <v>6.820512816076576</v>
+      </c>
+      <c r="AI39">
+        <f>-SUM(AI34:AI36)+AI37</f>
+        <v>4.6405128160765763</v>
+      </c>
+      <c r="AJ39">
+        <f>-SUM(AJ34:AJ36)+AJ37</f>
+        <v>20.92271492899523</v>
+      </c>
+      <c r="AK39">
+        <f>-SUM(AK34:AK36)+AK37</f>
+        <v>20.92271492899523</v>
+      </c>
+      <c r="AL39">
+        <f>-SUM(AL34:AL36)+AL37</f>
+        <v>20.92271492899523</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C6:AK9 AM6:AP9">
+  <conditionalFormatting sqref="C3:AL3 AN3">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:AL16">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:AL3">
     <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:AL4">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:AL18">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:AL2">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:AL23">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN6:AQ15 C6:AL15">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2236,8 +5001,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:AK3 AM3">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="C26:AL30">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2248,58 +5013,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:AK10">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="C34:AL37">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:AK3">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:AK4">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:AK12">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:AK2">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>

</xml_diff>

<commit_message>
BESS: Improved inverter: - voltage is now limited to Udc - current is limited to ratio defined in mask - PLL lost of sync time is increased to 4s to allow for ridethrough AsyncEthernet - fixed to allow better discrimination for received frame - to avoid receiving messages broadcasted by Opal New debounce implementation - using single integrator
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,17 +484,17 @@
   <dimension ref="A1:AM39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM23" sqref="A2:AM23"/>
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="43" width="4.77734375" customWidth="1"/>
+    <col min="3" max="43" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>-3</v>
@@ -643,7 +643,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -762,7 +762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -881,7 +881,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -2484,19 +2484,19 @@
         <v>-0.1</v>
       </c>
       <c r="S17">
-        <v>-0.16</v>
+        <v>-0.1</v>
       </c>
       <c r="T17">
+        <v>-0.1</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0.2</v>
+      </c>
+      <c r="W17">
         <v>-0.2</v>
-      </c>
-      <c r="U17">
-        <v>1</v>
-      </c>
-      <c r="V17">
-        <v>1</v>
-      </c>
-      <c r="W17">
-        <v>-1</v>
       </c>
       <c r="X17">
         <v>-1</v>
@@ -2547,7 +2547,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -2606,10 +2606,10 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="U18">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="V18">
         <v>-0.2</v>
@@ -2666,7 +2666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -3198,25 +3198,25 @@
         <v>0.4</v>
       </c>
       <c r="S23">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="T23">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="U23">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="V23">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="W23">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="X23">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="Y23">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="Z23">
         <v>0.4</v>
@@ -3261,15 +3261,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="S25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -3418,454 +3418,454 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>19</v>
       </c>
       <c r="C27">
-        <f>IF(OR(C3=0,C4=1),0,IF(C5=3,"GF",C2*0.9*80))</f>
+        <f t="shared" ref="C27:AL27" si="31">IF(OR(C3=0,C4=1),0,IF(C5=3,"GF",C2*0.9*80))</f>
         <v>0</v>
       </c>
       <c r="D27">
-        <f>IF(OR(D3=0,D4=1),0,IF(D5=3,"GF",D2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="E27">
-        <f>IF(OR(E3=0,E4=1),0,IF(E5=3,"GF",E2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="F27">
-        <f>IF(OR(F3=0,F4=1),0,IF(F5=3,"GF",F2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="G27">
-        <f>IF(OR(G3=0,G4=1),0,IF(G5=3,"GF",G2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H27">
-        <f>IF(OR(H3=0,H4=1),0,IF(H5=3,"GF",H2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="I27">
-        <f>IF(OR(I3=0,I4=1),0,IF(I5=3,"GF",I2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="J27">
-        <f>IF(OR(J3=0,J4=1),0,IF(J5=3,"GF",J2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K27" t="str">
-        <f>IF(OR(K3=0,K4=1),0,IF(K5=3,"GF",K2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="L27" t="str">
-        <f>IF(OR(L3=0,L4=1),0,IF(L5=3,"GF",L2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="M27" t="str">
-        <f>IF(OR(M3=0,M4=1),0,IF(M5=3,"GF",M2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="N27" t="str">
-        <f>IF(OR(N3=0,N4=1),0,IF(N5=3,"GF",N2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="O27" t="str">
-        <f>IF(OR(O3=0,O4=1),0,IF(O5=3,"GF",O2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="P27" t="str">
-        <f>IF(OR(P3=0,P4=1),0,IF(P5=3,"GF",P2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="Q27" t="str">
-        <f>IF(OR(Q3=0,Q4=1),0,IF(Q5=3,"GF",Q2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="R27" t="str">
-        <f>IF(OR(R3=0,R4=1),0,IF(R5=3,"GF",R2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="S27">
-        <f>IF(OR(S3=0,S4=1),0,IF(S5=3,"GF",S2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>7.2000000000000011</v>
       </c>
       <c r="T27">
-        <f>IF(OR(T3=0,T4=1),0,IF(T5=3,"GF",T2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>7.2000000000000011</v>
       </c>
       <c r="U27">
-        <f>IF(OR(U3=0,U4=1),0,IF(U5=3,"GF",U2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>36</v>
       </c>
       <c r="V27">
-        <f>IF(OR(V3=0,V4=1),0,IF(V5=3,"GF",V2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>36</v>
       </c>
       <c r="W27">
-        <f>IF(OR(W3=0,W4=1),0,IF(W5=3,"GF",W2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>72</v>
       </c>
       <c r="X27">
-        <f>IF(OR(X3=0,X4=1),0,IF(X5=3,"GF",X2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>72</v>
       </c>
       <c r="Y27">
-        <f>IF(OR(Y3=0,Y4=1),0,IF(Y5=3,"GF",Y2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="Z27">
-        <f>IF(OR(Z3=0,Z4=1),0,IF(Z5=3,"GF",Z2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AA27">
-        <f>IF(OR(AA3=0,AA4=1),0,IF(AA5=3,"GF",AA2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AB27">
-        <f>IF(OR(AB3=0,AB4=1),0,IF(AB5=3,"GF",AB2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AC27">
-        <f>IF(OR(AC3=0,AC4=1),0,IF(AC5=3,"GF",AC2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AD27">
-        <f>IF(OR(AD3=0,AD4=1),0,IF(AD5=3,"GF",AD2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>21.6</v>
       </c>
       <c r="AE27">
-        <f>IF(OR(AE3=0,AE4=1),0,IF(AE5=3,"GF",AE2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>21.6</v>
       </c>
       <c r="AF27">
-        <f>IF(OR(AF3=0,AF4=1),0,IF(AF5=3,"GF",AF2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>21.6</v>
       </c>
       <c r="AG27">
-        <f>IF(OR(AG3=0,AG4=1),0,IF(AG5=3,"GF",AG2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>21.6</v>
       </c>
       <c r="AH27">
-        <f>IF(OR(AH3=0,AH4=1),0,IF(AH5=3,"GF",AH2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>21.6</v>
       </c>
       <c r="AI27" t="str">
-        <f>IF(OR(AI3=0,AI4=1),0,IF(AI5=3,"GF",AI2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="AJ27" t="str">
-        <f>IF(OR(AJ3=0,AJ4=1),0,IF(AJ5=3,"GF",AJ2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="AK27" t="str">
-        <f>IF(OR(AK3=0,AK4=1),0,IF(AK5=3,"GF",AK2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>GF</v>
       </c>
       <c r="AL27">
-        <f>IF(OR(AL3=0,AL4=1),0,IF(AL5=3,"GF",AL2*0.9*80))</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>20</v>
       </c>
       <c r="C28">
-        <f>IF(OR(C16=0,C16=0),0,IF(C21=0,"GF",C17*250))</f>
+        <f t="shared" ref="C28:AL28" si="32">IF(OR(C16=0,C16=0),0,IF(C21=0,"GF",C17*250))</f>
         <v>0</v>
       </c>
       <c r="D28" t="str">
-        <f>IF(OR(D16=0,D16=0),0,IF(D21=0,"GF",D17*250))</f>
+        <f t="shared" si="32"/>
         <v>GF</v>
       </c>
       <c r="E28" t="str">
-        <f>IF(OR(E16=0,E16=0),0,IF(E21=0,"GF",E17*250))</f>
+        <f t="shared" si="32"/>
         <v>GF</v>
       </c>
       <c r="F28" t="str">
-        <f>IF(OR(F16=0,F16=0),0,IF(F21=0,"GF",F17*250))</f>
+        <f t="shared" si="32"/>
         <v>GF</v>
       </c>
       <c r="G28" t="str">
-        <f>IF(OR(G16=0,G16=0),0,IF(G21=0,"GF",G17*250))</f>
+        <f t="shared" si="32"/>
         <v>GF</v>
       </c>
       <c r="H28" t="str">
-        <f>IF(OR(H16=0,H16=0),0,IF(H21=0,"GF",H17*250))</f>
+        <f t="shared" si="32"/>
         <v>GF</v>
       </c>
       <c r="I28" t="str">
-        <f>IF(OR(I16=0,I16=0),0,IF(I21=0,"GF",I17*250))</f>
+        <f t="shared" si="32"/>
         <v>GF</v>
       </c>
       <c r="J28">
-        <f>IF(OR(J16=0,J16=0),0,IF(J21=0,"GF",J17*250))</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K28">
-        <f>IF(OR(K16=0,K16=0),0,IF(K21=0,"GF",K17*250))</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="L28">
-        <f>IF(OR(L16=0,L16=0),0,IF(L21=0,"GF",L17*250))</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M28">
-        <f>IF(OR(M16=0,M16=0),0,IF(M21=0,"GF",M17*250))</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N28">
-        <f>IF(OR(N16=0,N16=0),0,IF(N21=0,"GF",N17*250))</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O28">
-        <f>IF(OR(O16=0,O16=0),0,IF(O21=0,"GF",O17*250))</f>
+        <f t="shared" si="32"/>
         <v>40</v>
       </c>
       <c r="P28">
-        <f>IF(OR(P16=0,P16=0),0,IF(P21=0,"GF",P17*250))</f>
+        <f t="shared" si="32"/>
         <v>20</v>
       </c>
       <c r="Q28">
-        <f>IF(OR(Q16=0,Q16=0),0,IF(Q21=0,"GF",Q17*250))</f>
+        <f t="shared" si="32"/>
         <v>-20</v>
       </c>
       <c r="R28">
-        <f>IF(OR(R16=0,R16=0),0,IF(R21=0,"GF",R17*250))</f>
+        <f t="shared" si="32"/>
         <v>-25</v>
       </c>
       <c r="S28">
-        <f>IF(OR(S16=0,S16=0),0,IF(S21=0,"GF",S17*250))</f>
-        <v>-40</v>
+        <f t="shared" si="32"/>
+        <v>-25</v>
       </c>
       <c r="T28">
-        <f>IF(OR(T16=0,T16=0),0,IF(T21=0,"GF",T17*250))</f>
+        <f t="shared" si="32"/>
+        <v>-25</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="32"/>
+        <v>50</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="32"/>
         <v>-50</v>
       </c>
-      <c r="U28">
-        <f>IF(OR(U16=0,U16=0),0,IF(U21=0,"GF",U17*250))</f>
-        <v>250</v>
-      </c>
-      <c r="V28">
-        <f>IF(OR(V16=0,V16=0),0,IF(V21=0,"GF",V17*250))</f>
-        <v>250</v>
-      </c>
-      <c r="W28">
-        <f>IF(OR(W16=0,W16=0),0,IF(W21=0,"GF",W17*250))</f>
+      <c r="X28">
+        <f t="shared" si="32"/>
         <v>-250</v>
       </c>
-      <c r="X28">
-        <f>IF(OR(X16=0,X16=0),0,IF(X21=0,"GF",X17*250))</f>
+      <c r="Y28">
+        <f t="shared" si="32"/>
         <v>-250</v>
       </c>
-      <c r="Y28">
-        <f>IF(OR(Y16=0,Y16=0),0,IF(Y21=0,"GF",Y17*250))</f>
+      <c r="Z28">
+        <f t="shared" si="32"/>
+        <v>50</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="32"/>
+        <v>50</v>
+      </c>
+      <c r="AB28">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="32"/>
         <v>-250</v>
       </c>
-      <c r="Z28">
-        <f>IF(OR(Z16=0,Z16=0),0,IF(Z21=0,"GF",Z17*250))</f>
+      <c r="AE28">
+        <f t="shared" si="32"/>
+        <v>-250</v>
+      </c>
+      <c r="AF28">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AG28">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AH28">
+        <f t="shared" si="32"/>
+        <v>25</v>
+      </c>
+      <c r="AI28">
+        <f t="shared" si="32"/>
         <v>50</v>
       </c>
-      <c r="AA28">
-        <f>IF(OR(AA16=0,AA16=0),0,IF(AA21=0,"GF",AA17*250))</f>
-        <v>50</v>
-      </c>
-      <c r="AB28">
-        <f>IF(OR(AB16=0,AB16=0),0,IF(AB21=0,"GF",AB17*250))</f>
-        <v>0</v>
-      </c>
-      <c r="AC28">
-        <f>IF(OR(AC16=0,AC16=0),0,IF(AC21=0,"GF",AC17*250))</f>
-        <v>0</v>
-      </c>
-      <c r="AD28">
-        <f>IF(OR(AD16=0,AD16=0),0,IF(AD21=0,"GF",AD17*250))</f>
-        <v>-250</v>
-      </c>
-      <c r="AE28">
-        <f>IF(OR(AE16=0,AE16=0),0,IF(AE21=0,"GF",AE17*250))</f>
-        <v>-250</v>
-      </c>
-      <c r="AF28">
-        <f>IF(OR(AF16=0,AF16=0),0,IF(AF21=0,"GF",AF17*250))</f>
-        <v>0</v>
-      </c>
-      <c r="AG28">
-        <f>IF(OR(AG16=0,AG16=0),0,IF(AG21=0,"GF",AG17*250))</f>
-        <v>0</v>
-      </c>
-      <c r="AH28">
-        <f>IF(OR(AH16=0,AH16=0),0,IF(AH21=0,"GF",AH17*250))</f>
-        <v>25</v>
-      </c>
-      <c r="AI28">
-        <f>IF(OR(AI16=0,AI16=0),0,IF(AI21=0,"GF",AI17*250))</f>
-        <v>50</v>
-      </c>
       <c r="AJ28">
-        <f>IF(OR(AJ16=0,AJ16=0),0,IF(AJ21=0,"GF",AJ17*250))</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AK28">
-        <f>IF(OR(AK16=0,AK16=0),0,IF(AK21=0,"GF",AK17*250))</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AL28">
-        <f>IF(OR(AL16=0,AL16=0),0,IF(AL21=0,"GF",AL17*250))</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
       <c r="C29">
-        <f>IF(C22=0,0,C23*100)</f>
+        <f t="shared" ref="C29:AL29" si="33">IF(C22=0,0,C23*100)</f>
         <v>0</v>
       </c>
       <c r="D29">
-        <f>IF(D22=0,0,D23*100)</f>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="E29">
-        <f>IF(E22=0,0,E23*100)</f>
+        <f t="shared" si="33"/>
         <v>30</v>
       </c>
       <c r="F29">
-        <f>IF(F22=0,0,F23*100)</f>
+        <f t="shared" si="33"/>
         <v>70</v>
       </c>
       <c r="G29">
-        <f>IF(G22=0,0,G23*100)</f>
+        <f t="shared" si="33"/>
         <v>100</v>
       </c>
       <c r="H29">
-        <f>IF(H22=0,0,H23*100)</f>
+        <f t="shared" si="33"/>
         <v>50</v>
       </c>
       <c r="I29">
-        <f>IF(I22=0,0,I23*100)</f>
+        <f t="shared" si="33"/>
         <v>70</v>
       </c>
       <c r="J29">
-        <f>IF(J22=0,0,J23*100)</f>
+        <f t="shared" si="33"/>
         <v>70</v>
       </c>
       <c r="K29">
-        <f>IF(K22=0,0,K23*100)</f>
+        <f t="shared" si="33"/>
         <v>30</v>
       </c>
       <c r="L29">
-        <f>IF(L22=0,0,L23*100)</f>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="M29">
-        <f>IF(M22=0,0,M23*100)</f>
+        <f t="shared" si="33"/>
         <v>20</v>
       </c>
       <c r="N29">
-        <f>IF(N22=0,0,N23*100)</f>
+        <f t="shared" si="33"/>
         <v>30</v>
       </c>
       <c r="O29">
-        <f>IF(O22=0,0,O23*100)</f>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="P29">
-        <f>IF(P22=0,0,P23*100)</f>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="Q29">
-        <f>IF(Q22=0,0,Q23*100)</f>
+        <f t="shared" si="33"/>
         <v>30</v>
       </c>
       <c r="R29">
-        <f>IF(R22=0,0,R23*100)</f>
+        <f t="shared" si="33"/>
         <v>40</v>
       </c>
       <c r="S29">
-        <f>IF(S22=0,0,S23*100)</f>
-        <v>70</v>
+        <f t="shared" si="33"/>
+        <v>10</v>
       </c>
       <c r="T29">
-        <f>IF(T22=0,0,T23*100)</f>
-        <v>80</v>
+        <f t="shared" si="33"/>
+        <v>10</v>
       </c>
       <c r="U29">
-        <f>IF(U22=0,0,U23*100)</f>
-        <v>90</v>
+        <f t="shared" si="33"/>
+        <v>10</v>
       </c>
       <c r="V29">
-        <f>IF(V22=0,0,V23*100)</f>
+        <f t="shared" si="33"/>
+        <v>20</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="33"/>
+        <v>40</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="33"/>
         <v>100</v>
       </c>
-      <c r="W29">
-        <f>IF(W22=0,0,W23*100)</f>
-        <v>0</v>
-      </c>
-      <c r="X29">
-        <f>IF(X22=0,0,X23*100)</f>
-        <v>100</v>
-      </c>
-      <c r="Y29">
-        <f>IF(Y22=0,0,Y23*100)</f>
-        <v>70</v>
-      </c>
       <c r="Z29">
-        <f>IF(Z22=0,0,Z23*100)</f>
+        <f t="shared" si="33"/>
         <v>40</v>
       </c>
       <c r="AA29">
-        <f>IF(AA22=0,0,AA23*100)</f>
+        <f t="shared" si="33"/>
         <v>30</v>
       </c>
       <c r="AB29">
-        <f>IF(AB22=0,0,AB23*100)</f>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="AC29">
-        <f>IF(AC22=0,0,AC23*100)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AD29">
-        <f>IF(AD22=0,0,AD23*100)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AE29">
-        <f>IF(AE22=0,0,AE23*100)</f>
+        <f t="shared" si="33"/>
         <v>30</v>
       </c>
       <c r="AF29">
-        <f>IF(AF22=0,0,AF23*100)</f>
+        <f t="shared" si="33"/>
         <v>60</v>
       </c>
       <c r="AG29">
-        <f>IF(AG22=0,0,AG23*100)</f>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="AH29">
-        <f>IF(AH22=0,0,AH23*100)</f>
+        <f t="shared" si="33"/>
         <v>20</v>
       </c>
       <c r="AI29">
-        <f>IF(AI22=0,0,AI23*100)</f>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="AJ29">
-        <f>IF(AJ22=0,0,AJ23*100)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AK29">
-        <f>IF(AK22=0,0,AK23*100)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AL29">
-        <f>IF(AL22=0,0,AL23*100)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -3874,296 +3874,296 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <f t="shared" ref="D30:AL30" si="31">(IF(D8=2,0,3)+IF(D9=2,0,25)+IF(D10=2,0,10)+IF(D11=2,0,15)+IF(D13=2,0,20)+IF(D14=2,0,10)+IF(D15=2,0,20))*0.9</f>
+        <f t="shared" ref="D30:AL30" si="34">(IF(D8=2,0,3)+IF(D9=2,0,25)+IF(D10=2,0,10)+IF(D11=2,0,15)+IF(D13=2,0,20)+IF(D14=2,0,10)+IF(D15=2,0,20))*0.9</f>
         <v>0</v>
       </c>
       <c r="E30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>2.7</v>
       </c>
       <c r="F30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>25.2</v>
       </c>
       <c r="G30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>43.2</v>
       </c>
       <c r="H30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>61.2</v>
       </c>
       <c r="I30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>92.7</v>
       </c>
       <c r="J30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="K30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="L30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>22.5</v>
       </c>
       <c r="M30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>43.2</v>
       </c>
       <c r="N30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>61.2</v>
       </c>
       <c r="O30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>92.7</v>
       </c>
       <c r="P30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>92.7</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>38.700000000000003</v>
       </c>
       <c r="R30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>38.700000000000003</v>
       </c>
       <c r="S30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>38.700000000000003</v>
       </c>
       <c r="T30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>38.700000000000003</v>
       </c>
       <c r="U30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>92.7</v>
       </c>
       <c r="V30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>92.7</v>
       </c>
       <c r="W30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>61.2</v>
       </c>
       <c r="X30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>61.2</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>74.7</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>92.7</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>92.7</v>
       </c>
       <c r="AB30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>92.7</v>
       </c>
       <c r="AC30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>92.7</v>
       </c>
       <c r="AD30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>92.7</v>
       </c>
       <c r="AE30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>61.2</v>
       </c>
       <c r="AF30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>61.2</v>
       </c>
       <c r="AG30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>61.2</v>
       </c>
       <c r="AH30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>61.2</v>
       </c>
       <c r="AI30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>61.2</v>
       </c>
       <c r="AJ30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>43.2</v>
       </c>
       <c r="AK30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>43.2</v>
       </c>
       <c r="AL30">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>43.2</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="C32">
-        <f>-SUM(C26:C29)+C30</f>
+        <f t="shared" ref="C32:AL32" si="35">-SUM(C26:C29)+C30</f>
         <v>0</v>
       </c>
       <c r="D32">
-        <f>-SUM(D26:D29)+D30</f>
+        <f t="shared" si="35"/>
         <v>-5</v>
       </c>
       <c r="E32">
-        <f>-SUM(E26:E29)+E30</f>
+        <f t="shared" si="35"/>
         <v>-27.3</v>
       </c>
       <c r="F32">
-        <f>-SUM(F26:F29)+F30</f>
+        <f t="shared" si="35"/>
         <v>-44.8</v>
       </c>
       <c r="G32">
-        <f>-SUM(G26:G29)+G30</f>
+        <f t="shared" si="35"/>
         <v>-56.8</v>
       </c>
       <c r="H32">
-        <f>-SUM(H26:H29)+H30</f>
+        <f t="shared" si="35"/>
         <v>11.200000000000003</v>
       </c>
       <c r="I32">
-        <f>-SUM(I26:I29)+I30</f>
+        <f t="shared" si="35"/>
         <v>22.700000000000003</v>
       </c>
       <c r="J32">
-        <f>-SUM(J26:J29)+J30</f>
+        <f t="shared" si="35"/>
         <v>-70</v>
       </c>
       <c r="K32">
-        <f>-SUM(K26:K29)+K30</f>
+        <f t="shared" si="35"/>
         <v>-30</v>
       </c>
       <c r="L32">
-        <f>-SUM(L26:L29)+L30</f>
+        <f t="shared" si="35"/>
         <v>12.5</v>
       </c>
       <c r="M32">
-        <f>-SUM(M26:M29)+M30</f>
+        <f t="shared" si="35"/>
         <v>23.200000000000003</v>
       </c>
       <c r="N32">
-        <f>-SUM(N26:N29)+N30</f>
+        <f t="shared" si="35"/>
         <v>31.200000000000003</v>
       </c>
       <c r="O32">
-        <f>-SUM(O26:O29)+O30</f>
+        <f t="shared" si="35"/>
         <v>42.7</v>
       </c>
       <c r="P32">
-        <f>-SUM(P26:P29)+P30</f>
+        <f t="shared" si="35"/>
         <v>62.7</v>
       </c>
       <c r="Q32">
-        <f>-SUM(Q26:Q29)+Q30</f>
+        <f t="shared" si="35"/>
         <v>28.700000000000003</v>
       </c>
       <c r="R32">
-        <f>-SUM(R26:R29)+R30</f>
+        <f t="shared" si="35"/>
         <v>23.700000000000003</v>
       </c>
       <c r="S32">
-        <f>-SUM(S26:S29)+S30</f>
-        <v>1.5</v>
+        <f t="shared" si="35"/>
+        <v>46.5</v>
       </c>
       <c r="T32">
-        <f>-SUM(T26:T29)+T30</f>
-        <v>1.5</v>
+        <f t="shared" si="35"/>
+        <v>46.5</v>
       </c>
       <c r="U32">
-        <f>-SUM(U26:U29)+U30</f>
-        <v>-283.3</v>
+        <f t="shared" si="35"/>
+        <v>46.7</v>
       </c>
       <c r="V32">
-        <f>-SUM(V26:V29)+V30</f>
-        <v>-293.3</v>
+        <f t="shared" si="35"/>
+        <v>-13.299999999999997</v>
       </c>
       <c r="W32">
-        <f>-SUM(W26:W29)+W30</f>
-        <v>239.2</v>
+        <f t="shared" si="35"/>
+        <v>39.200000000000003</v>
       </c>
       <c r="X32">
-        <f>-SUM(X26:X29)+X30</f>
-        <v>139.19999999999999</v>
+        <f t="shared" si="35"/>
+        <v>199.2</v>
       </c>
       <c r="Y32">
-        <f>-SUM(Y26:Y29)+Y30</f>
-        <v>254.7</v>
+        <f t="shared" si="35"/>
+        <v>224.7</v>
       </c>
       <c r="Z32">
-        <f>-SUM(Z26:Z29)+Z30</f>
+        <f t="shared" si="35"/>
         <v>2.7000000000000028</v>
       </c>
       <c r="AA32">
-        <f>-SUM(AA26:AA29)+AA30</f>
+        <f t="shared" si="35"/>
         <v>12.700000000000003</v>
       </c>
       <c r="AB32">
-        <f>-SUM(AB26:AB29)+AB30</f>
+        <f t="shared" si="35"/>
         <v>82.7</v>
       </c>
       <c r="AC32">
-        <f>-SUM(AC26:AC29)+AC30</f>
+        <f t="shared" si="35"/>
         <v>92.7</v>
       </c>
       <c r="AD32">
-        <f>-SUM(AD26:AD29)+AD30</f>
+        <f t="shared" si="35"/>
         <v>321.10000000000002</v>
       </c>
       <c r="AE32">
-        <f>-SUM(AE26:AE29)+AE30</f>
+        <f t="shared" si="35"/>
         <v>259.60000000000002</v>
       </c>
       <c r="AF32">
-        <f>-SUM(AF26:AF29)+AF30</f>
+        <f t="shared" si="35"/>
         <v>-20.399999999999991</v>
       </c>
       <c r="AG32">
-        <f>-SUM(AG26:AG29)+AG30</f>
+        <f t="shared" si="35"/>
         <v>29.6</v>
       </c>
       <c r="AH32">
-        <f>-SUM(AH26:AH29)+AH30</f>
+        <f t="shared" si="35"/>
         <v>-5.3999999999999915</v>
       </c>
       <c r="AI32">
-        <f>-SUM(AI26:AI29)+AI30</f>
+        <f t="shared" si="35"/>
         <v>1.2000000000000028</v>
       </c>
       <c r="AJ32">
-        <f>-SUM(AJ26:AJ29)+AJ30</f>
+        <f t="shared" si="35"/>
         <v>43.2</v>
       </c>
       <c r="AK32">
-        <f>-SUM(AK26:AK29)+AK30</f>
+        <f t="shared" si="35"/>
         <v>43.2</v>
       </c>
       <c r="AL32">
-        <f>-SUM(AL26:AL29)+AL30</f>
+        <f t="shared" si="35"/>
         <v>43.2</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -4172,147 +4172,147 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:AL34" si="32">IF(OR(D3=0,D4=1),0,IF(D5=3,"GF",D2*0.43*80))</f>
+        <f t="shared" ref="D34:AL34" si="36">IF(OR(D3=0,D4=1),0,IF(D5=3,"GF",D2*0.43*80))</f>
         <v>0</v>
       </c>
       <c r="E34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="G34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="H34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="I34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="J34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="R34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="S34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>3.4400000000000004</v>
       </c>
       <c r="T34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>3.4400000000000004</v>
       </c>
       <c r="U34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>17.2</v>
       </c>
       <c r="V34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>17.2</v>
       </c>
       <c r="W34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>34.4</v>
       </c>
       <c r="X34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>34.4</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AA34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AB34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AC34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AD34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>10.32</v>
       </c>
       <c r="AE34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>10.32</v>
       </c>
       <c r="AF34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>10.32</v>
       </c>
       <c r="AG34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>10.32</v>
       </c>
       <c r="AH34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>10.32</v>
       </c>
       <c r="AI34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="AJ34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="AK34" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>GF</v>
       </c>
       <c r="AL34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -4321,296 +4321,296 @@
         <v>0</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" ref="D35:AL35" si="33">IF(OR(D16=0,D16=0),0,IF(D21=0,"GF",D18*250))</f>
+        <f t="shared" ref="D35:AL35" si="37">IF(OR(D16=0,D16=0),0,IF(D21=0,"GF",D18*250))</f>
         <v>GF</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>GF</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>GF</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>GF</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>GF</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>GF</v>
       </c>
       <c r="J35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="L35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="M35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="N35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="O35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>25</v>
       </c>
       <c r="P35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>25</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>12.5</v>
       </c>
       <c r="R35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="S35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="T35">
-        <f t="shared" si="33"/>
-        <v>50</v>
+        <f t="shared" si="37"/>
+        <v>0</v>
       </c>
       <c r="U35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="37"/>
         <v>-50</v>
       </c>
-      <c r="V35">
-        <f t="shared" si="33"/>
+      <c r="W35">
+        <f t="shared" si="37"/>
         <v>-50</v>
       </c>
-      <c r="W35">
-        <f t="shared" si="33"/>
+      <c r="X35">
+        <f t="shared" si="37"/>
         <v>-50</v>
       </c>
-      <c r="X35">
-        <f t="shared" si="33"/>
+      <c r="Y35">
+        <f t="shared" si="37"/>
         <v>-50</v>
       </c>
-      <c r="Y35">
-        <f t="shared" si="33"/>
-        <v>-50</v>
-      </c>
       <c r="Z35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AA35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AB35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AC35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AD35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AE35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AF35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AG35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AH35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>12.5</v>
       </c>
       <c r="AI35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>25</v>
       </c>
       <c r="AJ35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AK35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AL35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>21</v>
       </c>
       <c r="C36">
-        <f>IF(C30=0,0,C31*100)</f>
+        <f t="shared" ref="C36:AL36" si="38">IF(C30=0,0,C31*100)</f>
         <v>0</v>
       </c>
       <c r="D36">
-        <f>IF(D30=0,0,D31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="E36">
-        <f>IF(E30=0,0,E31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="F36">
-        <f>IF(F30=0,0,F31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G36">
-        <f>IF(G30=0,0,G31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="H36">
-        <f>IF(H30=0,0,H31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="I36">
-        <f>IF(I30=0,0,I31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="J36">
-        <f>IF(J30=0,0,J31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="K36">
-        <f>IF(K30=0,0,K31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="L36">
-        <f>IF(L30=0,0,L31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="M36">
-        <f>IF(M30=0,0,M31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="N36">
-        <f>IF(N30=0,0,N31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O36">
-        <f>IF(O30=0,0,O31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="P36">
-        <f>IF(P30=0,0,P31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Q36">
-        <f>IF(Q30=0,0,Q31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R36">
-        <f>IF(R30=0,0,R31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="S36">
-        <f>IF(S30=0,0,S31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="T36">
-        <f>IF(T30=0,0,T31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="U36">
-        <f>IF(U30=0,0,U31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="V36">
-        <f>IF(V30=0,0,V31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="W36">
-        <f>IF(W30=0,0,W31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X36">
-        <f>IF(X30=0,0,X31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Y36">
-        <f>IF(Y30=0,0,Y31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Z36">
-        <f>IF(Z30=0,0,Z31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AA36">
-        <f>IF(AA30=0,0,AA31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB36">
-        <f>IF(AB30=0,0,AB31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AC36">
-        <f>IF(AC30=0,0,AC31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AD36">
-        <f>IF(AD30=0,0,AD31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AE36">
-        <f>IF(AE30=0,0,AE31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AF36">
-        <f>IF(AF30=0,0,AF31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AG36">
-        <f>IF(AG30=0,0,AG31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AH36">
-        <f>IF(AH30=0,0,AH31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AI36">
-        <f>IF(AI30=0,0,AI31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AJ36">
-        <f>IF(AJ30=0,0,AJ31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AK36">
-        <f>IF(AK30=0,0,AK31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AL36">
-        <f>IF(AL30=0,0,AL31*100)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -4619,147 +4619,147 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:AL37" si="34">(IF(D8=2,0,3)+IF(D9=2,0,25)+IF(D10=2,0,10)+IF(D11=2,0,15)+IF(D13=2,0,20)+IF(D14=2,0,10)+IF(D15=2,0,20))*(SQRT(1-(0.9*0.9)))</f>
+        <f t="shared" ref="D37:AL37" si="39">(IF(D8=2,0,3)+IF(D9=2,0,25)+IF(D10=2,0,10)+IF(D11=2,0,15)+IF(D13=2,0,20)+IF(D14=2,0,10)+IF(D15=2,0,20))*(SQRT(1-(0.9*0.9)))</f>
         <v>0</v>
       </c>
       <c r="E37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>1.3076696830622019</v>
       </c>
       <c r="F37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>12.204917041913884</v>
       </c>
       <c r="G37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>20.92271492899523</v>
       </c>
       <c r="H37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>29.640512816076576</v>
       </c>
       <c r="I37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>44.896659118468932</v>
       </c>
       <c r="J37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="K37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="L37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>10.897247358851683</v>
       </c>
       <c r="M37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>20.92271492899523</v>
       </c>
       <c r="N37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>29.640512816076576</v>
       </c>
       <c r="O37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>44.896659118468932</v>
       </c>
       <c r="P37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>44.896659118468932</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>18.743265457224894</v>
       </c>
       <c r="R37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>18.743265457224894</v>
       </c>
       <c r="S37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>18.743265457224894</v>
       </c>
       <c r="T37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>18.743265457224894</v>
       </c>
       <c r="U37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>44.896659118468932</v>
       </c>
       <c r="V37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>44.896659118468932</v>
       </c>
       <c r="W37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>29.640512816076576</v>
       </c>
       <c r="X37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>29.640512816076576</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>36.178861231387586</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>44.896659118468932</v>
       </c>
       <c r="AA37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>44.896659118468932</v>
       </c>
       <c r="AB37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>44.896659118468932</v>
       </c>
       <c r="AC37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>44.896659118468932</v>
       </c>
       <c r="AD37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>44.896659118468932</v>
       </c>
       <c r="AE37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>29.640512816076576</v>
       </c>
       <c r="AF37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>29.640512816076576</v>
       </c>
       <c r="AG37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>29.640512816076576</v>
       </c>
       <c r="AH37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>29.640512816076576</v>
       </c>
       <c r="AI37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>29.640512816076576</v>
       </c>
       <c r="AJ37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>20.92271492899523</v>
       </c>
       <c r="AK37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>20.92271492899523</v>
       </c>
       <c r="AL37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>20.92271492899523</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -4768,143 +4768,143 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <f>-SUM(D34:D36)+D37</f>
+        <f t="shared" ref="D39:AL39" si="40">-SUM(D34:D36)+D37</f>
         <v>0</v>
       </c>
       <c r="E39">
-        <f>-SUM(E34:E36)+E37</f>
+        <f t="shared" si="40"/>
         <v>1.3076696830622019</v>
       </c>
       <c r="F39">
-        <f>-SUM(F34:F36)+F37</f>
+        <f t="shared" si="40"/>
         <v>12.204917041913884</v>
       </c>
       <c r="G39">
-        <f>-SUM(G34:G36)+G37</f>
+        <f t="shared" si="40"/>
         <v>20.92271492899523</v>
       </c>
       <c r="H39">
-        <f>-SUM(H34:H36)+H37</f>
+        <f t="shared" si="40"/>
         <v>29.640512816076576</v>
       </c>
       <c r="I39">
-        <f>-SUM(I34:I36)+I37</f>
+        <f t="shared" si="40"/>
         <v>44.896659118468932</v>
       </c>
       <c r="J39">
-        <f>-SUM(J34:J36)+J37</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K39">
-        <f>-SUM(K34:K36)+K37</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="L39">
-        <f>-SUM(L34:L36)+L37</f>
+        <f t="shared" si="40"/>
         <v>10.897247358851683</v>
       </c>
       <c r="M39">
-        <f>-SUM(M34:M36)+M37</f>
+        <f t="shared" si="40"/>
         <v>20.92271492899523</v>
       </c>
       <c r="N39">
-        <f>-SUM(N34:N36)+N37</f>
+        <f t="shared" si="40"/>
         <v>29.640512816076576</v>
       </c>
       <c r="O39">
-        <f>-SUM(O34:O36)+O37</f>
+        <f t="shared" si="40"/>
         <v>19.896659118468932</v>
       </c>
       <c r="P39">
-        <f>-SUM(P34:P36)+P37</f>
+        <f t="shared" si="40"/>
         <v>19.896659118468932</v>
       </c>
       <c r="Q39">
-        <f>-SUM(Q34:Q36)+Q37</f>
+        <f t="shared" si="40"/>
         <v>6.2432654572248936</v>
       </c>
       <c r="R39">
-        <f>-SUM(R34:R36)+R37</f>
+        <f t="shared" si="40"/>
         <v>18.743265457224894</v>
       </c>
       <c r="S39">
-        <f>-SUM(S34:S36)+S37</f>
+        <f t="shared" si="40"/>
         <v>15.303265457224892</v>
       </c>
       <c r="T39">
-        <f>-SUM(T34:T36)+T37</f>
-        <v>-34.696734542775104</v>
+        <f t="shared" si="40"/>
+        <v>15.303265457224892</v>
       </c>
       <c r="U39">
-        <f>-SUM(U34:U36)+U37</f>
+        <f t="shared" si="40"/>
+        <v>27.696659118468933</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="40"/>
         <v>77.696659118468929</v>
       </c>
-      <c r="V39">
-        <f>-SUM(V34:V36)+V37</f>
-        <v>77.696659118468929</v>
-      </c>
       <c r="W39">
-        <f>-SUM(W34:W36)+W37</f>
+        <f t="shared" si="40"/>
         <v>45.240512816076574</v>
       </c>
       <c r="X39">
-        <f>-SUM(X34:X36)+X37</f>
+        <f t="shared" si="40"/>
         <v>45.240512816076574</v>
       </c>
       <c r="Y39">
-        <f>-SUM(Y34:Y36)+Y37</f>
+        <f t="shared" si="40"/>
         <v>86.178861231387586</v>
       </c>
       <c r="Z39">
-        <f>-SUM(Z34:Z36)+Z37</f>
+        <f t="shared" si="40"/>
         <v>44.896659118468932</v>
       </c>
       <c r="AA39">
-        <f>-SUM(AA34:AA36)+AA37</f>
+        <f t="shared" si="40"/>
         <v>44.896659118468932</v>
       </c>
       <c r="AB39">
-        <f>-SUM(AB34:AB36)+AB37</f>
+        <f t="shared" si="40"/>
         <v>44.896659118468932</v>
       </c>
       <c r="AC39">
-        <f>-SUM(AC34:AC36)+AC37</f>
+        <f t="shared" si="40"/>
         <v>44.896659118468932</v>
       </c>
       <c r="AD39">
-        <f>-SUM(AD34:AD36)+AD37</f>
+        <f t="shared" si="40"/>
         <v>34.576659118468932</v>
       </c>
       <c r="AE39">
-        <f>-SUM(AE34:AE36)+AE37</f>
+        <f t="shared" si="40"/>
         <v>19.320512816076576</v>
       </c>
       <c r="AF39">
-        <f>-SUM(AF34:AF36)+AF37</f>
+        <f t="shared" si="40"/>
         <v>19.320512816076576</v>
       </c>
       <c r="AG39">
-        <f>-SUM(AG34:AG36)+AG37</f>
+        <f t="shared" si="40"/>
         <v>19.320512816076576</v>
       </c>
       <c r="AH39">
-        <f>-SUM(AH34:AH36)+AH37</f>
+        <f t="shared" si="40"/>
         <v>6.820512816076576</v>
       </c>
       <c r="AI39">
-        <f>-SUM(AI34:AI36)+AI37</f>
+        <f t="shared" si="40"/>
         <v>4.6405128160765763</v>
       </c>
       <c r="AJ39">
-        <f>-SUM(AJ34:AJ36)+AJ37</f>
+        <f t="shared" si="40"/>
         <v>20.92271492899523</v>
       </c>
       <c r="AK39">
-        <f>-SUM(AK34:AK36)+AK37</f>
+        <f t="shared" si="40"/>
         <v>20.92271492899523</v>
       </c>
       <c r="AL39">
-        <f>-SUM(AL34:AL36)+AL37</f>
+        <f t="shared" si="40"/>
         <v>20.92271492899523</v>
       </c>
     </row>
@@ -5036,7 +5036,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5048,7 +5048,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed stimuli pattern for better stability Added links opening script to BANSHEE_init.m - only works with Opal -> needs variable initialisation befoere opening model: OpenLinks=1;
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
@@ -484,7 +484,7 @@
   <dimension ref="A1:AM39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,150 +497,150 @@
     <row r="1" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="C1" s="1">
         <v>0</v>
       </c>
       <c r="D1">
         <f>C1+C1-B1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1">
         <f>D1+D1-C1</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1">
         <f t="shared" ref="F1:I1" si="0">E1+E1-D1</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H1">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I1">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J1">
         <f t="shared" ref="J1" si="1">I1+I1-H1</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="K1">
         <f t="shared" ref="K1" si="2">J1+J1-I1</f>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="L1">
         <f t="shared" ref="L1" si="3">K1+K1-J1</f>
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="M1">
         <f t="shared" ref="M1" si="4">L1+L1-K1</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="N1">
         <f t="shared" ref="N1" si="5">M1+M1-L1</f>
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="O1">
         <f t="shared" ref="O1" si="6">N1+N1-M1</f>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="P1">
         <f t="shared" ref="P1" si="7">O1+O1-N1</f>
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="Q1">
         <f t="shared" ref="Q1" si="8">P1+P1-O1</f>
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="R1">
         <f t="shared" ref="R1" si="9">Q1+Q1-P1</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="S1">
         <f t="shared" ref="S1" si="10">R1+R1-Q1</f>
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="T1">
         <f t="shared" ref="T1" si="11">S1+S1-R1</f>
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="U1">
         <f t="shared" ref="U1" si="12">T1+T1-S1</f>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="V1">
         <f t="shared" ref="V1" si="13">U1+U1-T1</f>
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="W1">
         <f t="shared" ref="W1" si="14">V1+V1-U1</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="X1">
         <f t="shared" ref="X1" si="15">W1+W1-V1</f>
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="Y1">
         <f t="shared" ref="Y1" si="16">X1+X1-W1</f>
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="Z1">
         <f t="shared" ref="Z1" si="17">Y1+Y1-X1</f>
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="AA1">
         <f t="shared" ref="AA1" si="18">Z1+Z1-Y1</f>
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="AB1">
         <f t="shared" ref="AB1" si="19">AA1+AA1-Z1</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="AC1">
         <f t="shared" ref="AC1" si="20">AB1+AB1-AA1</f>
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="AD1">
         <f t="shared" ref="AD1" si="21">AC1+AC1-AB1</f>
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="AE1">
         <f t="shared" ref="AE1" si="22">AD1+AD1-AC1</f>
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="AF1">
         <f t="shared" ref="AF1" si="23">AE1+AE1-AD1</f>
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="AG1">
         <f t="shared" ref="AG1" si="24">AF1+AF1-AE1</f>
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="AH1">
         <f t="shared" ref="AH1" si="25">AG1+AG1-AF1</f>
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="AI1">
         <f t="shared" ref="AI1" si="26">AH1+AH1-AG1</f>
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="AJ1">
         <f t="shared" ref="AJ1" si="27">AI1+AI1-AH1</f>
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="AK1">
         <f t="shared" ref="AK1" si="28">AJ1+AJ1-AI1</f>
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="AL1">
         <f t="shared" ref="AL1" si="29">AK1+AK1-AJ1</f>
-        <v>105</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -2234,7 +2234,7 @@
         <v>2</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P15">
         <v>1</v>
@@ -2472,10 +2472,10 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="Q17">
         <v>-0.08</v>
@@ -2591,10 +2591,10 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P18">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="Q18">
         <v>0.05</v>
@@ -3180,16 +3180,16 @@
         <v>0.1</v>
       </c>
       <c r="M23">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="N23">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="O23">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P23">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="Q23">
         <v>0.3</v>
@@ -3621,11 +3621,11 @@
       </c>
       <c r="O28">
         <f t="shared" si="32"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="P28">
         <f t="shared" si="32"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q28">
         <f t="shared" si="32"/>
@@ -3762,19 +3762,19 @@
       </c>
       <c r="M29">
         <f t="shared" si="33"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N29">
         <f t="shared" si="33"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O29">
         <f t="shared" si="33"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P29">
         <f t="shared" si="33"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q29">
         <f t="shared" si="33"/>
@@ -3919,7 +3919,7 @@
       </c>
       <c r="O30">
         <f t="shared" si="34"/>
-        <v>92.7</v>
+        <v>74.7</v>
       </c>
       <c r="P30">
         <f t="shared" si="34"/>
@@ -4060,19 +4060,19 @@
       </c>
       <c r="M32">
         <f t="shared" si="35"/>
-        <v>23.200000000000003</v>
+        <v>43.2</v>
       </c>
       <c r="N32">
         <f t="shared" si="35"/>
-        <v>31.200000000000003</v>
+        <v>61.2</v>
       </c>
       <c r="O32">
         <f t="shared" si="35"/>
-        <v>42.7</v>
+        <v>74.7</v>
       </c>
       <c r="P32">
         <f t="shared" si="35"/>
-        <v>62.7</v>
+        <v>92.7</v>
       </c>
       <c r="Q32">
         <f t="shared" si="35"/>
@@ -4366,11 +4366,11 @@
       </c>
       <c r="O35">
         <f t="shared" si="37"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="P35">
         <f t="shared" si="37"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q35">
         <f t="shared" si="37"/>
@@ -4664,7 +4664,7 @@
       </c>
       <c r="O37">
         <f t="shared" si="39"/>
-        <v>44.896659118468932</v>
+        <v>36.178861231387586</v>
       </c>
       <c r="P37">
         <f t="shared" si="39"/>
@@ -4813,11 +4813,11 @@
       </c>
       <c r="O39">
         <f t="shared" si="40"/>
-        <v>19.896659118468932</v>
+        <v>36.178861231387586</v>
       </c>
       <c r="P39">
         <f t="shared" si="40"/>
-        <v>19.896659118468932</v>
+        <v>44.896659118468932</v>
       </c>
       <c r="Q39">
         <f t="shared" si="40"/>

</xml_diff>

<commit_message>
Updated ESS2 with new inverter model Added - battery level limitations in ESS mode - will trip when in VF mode and batt low/full.
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
@@ -57,9 +57,6 @@
     <t>Stim.ESS2.f</t>
   </si>
   <si>
-    <t>Stim.ESS2.MCB</t>
-  </si>
-  <si>
     <t>= [</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>GenQ</t>
+  </si>
+  <si>
+    <t>Stim.ESS2.VFmode</t>
   </si>
 </sst>
 </file>
@@ -484,12 +484,12 @@
   <dimension ref="A1:AM39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="C35" sqref="C35:AL35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
     <col min="3" max="43" width="4.7109375" customWidth="1"/>
   </cols>
@@ -648,7 +648,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>0.1</v>
@@ -759,7 +759,7 @@
         <v>0.3</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -767,7 +767,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="AM3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -886,7 +886,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -997,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -1005,7 +1005,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -1116,7 +1116,7 @@
         <v>3</v>
       </c>
       <c r="AM5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1235,7 +1235,7 @@
         <v>2</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -1243,7 +1243,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1354,15 +1354,15 @@
         <v>2</v>
       </c>
       <c r="AM7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
       <c r="AM8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -1481,7 +1481,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1592,15 +1592,15 @@
         <v>1</v>
       </c>
       <c r="AM9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1711,15 +1711,15 @@
         <v>2</v>
       </c>
       <c r="AM10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1830,15 +1830,15 @@
         <v>2</v>
       </c>
       <c r="AM11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1949,7 +1949,7 @@
         <v>1</v>
       </c>
       <c r="AM12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -1957,7 +1957,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -2068,15 +2068,15 @@
         <v>1</v>
       </c>
       <c r="AM13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -2187,15 +2187,15 @@
         <v>2</v>
       </c>
       <c r="AM14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -2306,7 +2306,7 @@
         <v>2</v>
       </c>
       <c r="AM15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -2314,7 +2314,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2425,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="AM16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -2433,7 +2433,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2544,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="AM17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -2552,7 +2552,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="AM18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -2671,7 +2671,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2782,7 +2782,7 @@
         <v>1</v>
       </c>
       <c r="AM19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -2790,7 +2790,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2901,134 +2901,134 @@
         <v>1</v>
       </c>
       <c r="AM20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -3139,15 +3139,15 @@
         <v>1</v>
       </c>
       <c r="AM22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -3258,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="AM23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
@@ -3266,12 +3266,12 @@
     </row>
     <row r="25" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="S25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26">
         <f>IF(C6=2,0,"GF")</f>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="27" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27">
         <f t="shared" ref="C27:AL27" si="31">IF(OR(C3=0,C4=1),0,IF(C5=3,"GF",C2*0.9*80))</f>
@@ -3569,14 +3569,14 @@
     </row>
     <row r="28" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:AL28" si="32">IF(OR(C16=0,C16=0),0,IF(C21=0,"GF",C17*250))</f>
+        <f>IF(OR(C16=0,C16=0),0,IF(C21=1,"GF",C17*250))</f>
         <v>0</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="D28:AL28" si="32">IF(OR(D16=0,D16=0),0,IF(D21=1,"GF",D17*250))</f>
         <v>GF</v>
       </c>
       <c r="E28" t="str">
@@ -3718,7 +3718,7 @@
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29">
         <f t="shared" ref="C29:AL29" si="33">IF(C22=0,0,C23*100)</f>
@@ -3867,7 +3867,7 @@
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30">
         <f>(IF(C8=2,0,3)+IF(C9=2,0,25)+IF(C10=2,0,10)+IF(C11=2,0,15)+IF(C13=2,0,20)+IF(C14=2,0,10)+IF(C15=2,0,20))*0.9</f>
@@ -4016,7 +4016,7 @@
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32">
         <f t="shared" ref="C32:AL32" si="35">-SUM(C26:C29)+C30</f>
@@ -4165,7 +4165,7 @@
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34">
         <f>IF(OR(C3=0,C4=1),0,IF(C5=3,"GF",C2*0.43*80))</f>
@@ -4314,14 +4314,14 @@
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35">
-        <f>IF(OR(C16=0,C16=0),0,IF(C21=0,"GF",C18*250))</f>
+        <f>IF(OR(C16=0,C16=0),0,IF(C21=1,"GF",C18*250))</f>
         <v>0</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" ref="D35:AL35" si="37">IF(OR(D16=0,D16=0),0,IF(D21=0,"GF",D18*250))</f>
+        <f t="shared" ref="D35:AL35" si="37">IF(OR(D16=0,D16=0),0,IF(D21=1,"GF",D18*250))</f>
         <v>GF</v>
       </c>
       <c r="E35" t="str">
@@ -4463,7 +4463,7 @@
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36">
         <f t="shared" ref="C36:AL36" si="38">IF(C30=0,0,C31*100)</f>
@@ -4612,7 +4612,7 @@
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37">
         <f>(IF(C8=2,0,3)+IF(C9=2,0,25)+IF(C10=2,0,10)+IF(C11=2,0,15)+IF(C13=2,0,20)+IF(C14=2,0,10)+IF(C15=2,0,20))*(SQRT(1-(0.9*0.9)))</f>
@@ -4761,7 +4761,7 @@
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C39">
         <f>(IF(C8=2,0,3)+IF(C9=2,0,25)+IF(C10=2,0,10)+IF(C11=2,0,15)+IF(C13=2,0,20)+IF(C14=2,0,10)+IF(C15=2,0,20))*(SQRT(1-(0.9*0.9)))</f>

</xml_diff>

<commit_message>
BESS_lib.mdl - added latch model - not in inverter yet Remote chill - changed modbus TCP config - different slave ID's Openned link for relay in ESS
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
@@ -66,9 +66,6 @@
     <t>];</t>
   </si>
   <si>
-    <t>Stim.PV.p</t>
-  </si>
-  <si>
     <t>Stim.PV.Ena</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>Stim.ESS2.VFmode</t>
+  </si>
+  <si>
+    <t>Stim.PV.Irradiance</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:AM39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:AL35"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="8" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="10" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>13</v>
@@ -1716,7 +1716,7 @@
     </row>
     <row r="11" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="12" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="14" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="15" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="21" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>13</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="22" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
@@ -3144,7 +3144,7 @@
     </row>
     <row r="23" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>13</v>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="26" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <f>IF(C6=2,0,"GF")</f>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="27" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27">
         <f t="shared" ref="C27:AL27" si="31">IF(OR(C3=0,C4=1),0,IF(C5=3,"GF",C2*0.9*80))</f>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="28" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28">
         <f>IF(OR(C16=0,C16=0),0,IF(C21=1,"GF",C17*250))</f>
@@ -3718,7 +3718,7 @@
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29">
         <f t="shared" ref="C29:AL29" si="33">IF(C22=0,0,C23*100)</f>
@@ -3867,7 +3867,7 @@
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30">
         <f>(IF(C8=2,0,3)+IF(C9=2,0,25)+IF(C10=2,0,10)+IF(C11=2,0,15)+IF(C13=2,0,20)+IF(C14=2,0,10)+IF(C15=2,0,20))*0.9</f>
@@ -4016,7 +4016,7 @@
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32">
         <f t="shared" ref="C32:AL32" si="35">-SUM(C26:C29)+C30</f>
@@ -4165,7 +4165,7 @@
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C34">
         <f>IF(OR(C3=0,C4=1),0,IF(C5=3,"GF",C2*0.43*80))</f>
@@ -4314,7 +4314,7 @@
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35">
         <f>IF(OR(C16=0,C16=0),0,IF(C21=1,"GF",C18*250))</f>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36">
         <f t="shared" ref="C36:AL36" si="38">IF(C30=0,0,C31*100)</f>
@@ -4612,7 +4612,7 @@
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C37">
         <f>(IF(C8=2,0,3)+IF(C9=2,0,25)+IF(C10=2,0,10)+IF(C11=2,0,15)+IF(C13=2,0,20)+IF(C14=2,0,10)+IF(C15=2,0,20))*(SQRT(1-(0.9*0.9)))</f>
@@ -4761,7 +4761,7 @@
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39">
         <f>(IF(C8=2,0,3)+IF(C9=2,0,25)+IF(C10=2,0,10)+IF(C11=2,0,15)+IF(C13=2,0,20)+IF(C14=2,0,10)+IF(C15=2,0,20))*(SQRT(1-(0.9*0.9)))</f>

</xml_diff>

<commit_message>
Added PHIL node Added F3 relay 10
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/Stimuli.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="89">
   <si>
     <t>Stim.CB.CB401</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Stim.PV2.Irradiance</t>
+  </si>
+  <si>
+    <t>Stim.CB.CB310</t>
   </si>
 </sst>
 </file>
@@ -4605,10 +4608,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM77"/>
+  <dimension ref="A1:AM78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A77" sqref="A2:XFD77"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11193,13 +11196,13 @@
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56">
         <v>2</v>
@@ -11247,52 +11250,52 @@
         <v>2</v>
       </c>
       <c r="S56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI56">
         <v>2</v>
@@ -11312,7 +11315,7 @@
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>10</v>
@@ -11333,10 +11336,10 @@
         <v>2</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J57">
         <v>2</v>
@@ -11351,19 +11354,19 @@
         <v>2</v>
       </c>
       <c r="N57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S57">
         <v>1</v>
@@ -11414,7 +11417,7 @@
         <v>1</v>
       </c>
       <c r="AI57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ57">
         <v>2</v>
@@ -11431,7 +11434,7 @@
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>10</v>
@@ -11452,7 +11455,7 @@
         <v>2</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <v>1</v>
@@ -11470,7 +11473,7 @@
         <v>2</v>
       </c>
       <c r="N58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O58">
         <v>1</v>
@@ -11479,16 +11482,16 @@
         <v>1</v>
       </c>
       <c r="Q58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U58">
         <v>1</v>
@@ -11497,10 +11500,10 @@
         <v>1</v>
       </c>
       <c r="W58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y58">
         <v>1</v>
@@ -11521,19 +11524,19 @@
         <v>1</v>
       </c>
       <c r="AE58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ58">
         <v>2</v>
@@ -11550,7 +11553,7 @@
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>10</v>
@@ -11565,13 +11568,13 @@
         <v>2</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I59">
         <v>1</v>
@@ -11583,13 +11586,13 @@
         <v>2</v>
       </c>
       <c r="L59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O59">
         <v>1</v>
@@ -11598,16 +11601,16 @@
         <v>1</v>
       </c>
       <c r="Q59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U59">
         <v>1</v>
@@ -11616,10 +11619,10 @@
         <v>1</v>
       </c>
       <c r="W59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y59">
         <v>1</v>
@@ -11640,28 +11643,28 @@
         <v>1</v>
       </c>
       <c r="AE59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM59" s="2" t="s">
         <v>12</v>
@@ -11669,7 +11672,7 @@
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>10</v>
@@ -11684,10 +11687,10 @@
         <v>2</v>
       </c>
       <c r="F60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -11702,10 +11705,10 @@
         <v>2</v>
       </c>
       <c r="L60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N60">
         <v>1</v>
@@ -11774,13 +11777,13 @@
         <v>1</v>
       </c>
       <c r="AJ60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM60" s="2" t="s">
         <v>12</v>
@@ -11788,7 +11791,7 @@
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>10</v>
@@ -11809,7 +11812,7 @@
         <v>2</v>
       </c>
       <c r="H61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I61">
         <v>1</v>
@@ -11827,25 +11830,25 @@
         <v>2</v>
       </c>
       <c r="N61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P61">
         <v>1</v>
       </c>
       <c r="Q61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U61">
         <v>1</v>
@@ -11854,13 +11857,13 @@
         <v>1</v>
       </c>
       <c r="W61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z61">
         <v>1</v>
@@ -11878,19 +11881,19 @@
         <v>1</v>
       </c>
       <c r="AE61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ61">
         <v>2</v>
@@ -11907,64 +11910,64 @@
     </row>
     <row r="62" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I62">
         <v>1</v>
       </c>
       <c r="J62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P62">
         <v>1</v>
       </c>
       <c r="Q62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U62">
         <v>1</v>
@@ -11973,13 +11976,13 @@
         <v>1</v>
       </c>
       <c r="W62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z62">
         <v>1</v>
@@ -11988,37 +11991,37 @@
         <v>1</v>
       </c>
       <c r="AB62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD62">
         <v>1</v>
       </c>
       <c r="AE62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM62" s="2" t="s">
         <v>12</v>
@@ -12026,7 +12029,7 @@
     </row>
     <row r="63" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>10</v>
@@ -12035,22 +12038,22 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63">
         <v>0</v>
@@ -12059,79 +12062,79 @@
         <v>0</v>
       </c>
       <c r="L63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q63">
-        <v>-0.08</v>
+        <v>1</v>
       </c>
       <c r="R63">
-        <v>-0.1</v>
+        <v>1</v>
       </c>
       <c r="S63">
-        <v>-0.1</v>
+        <v>1</v>
       </c>
       <c r="T63">
-        <v>-0.1</v>
+        <v>1</v>
       </c>
       <c r="U63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V63">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="W63">
-        <v>-0.2</v>
+        <v>1</v>
       </c>
       <c r="X63">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y63">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z63">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AA63">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AB63">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC63">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD63">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AE63">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AF63">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AG63">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AH63">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="AI63">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AJ63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK63">
         <v>0</v>
@@ -12145,7 +12148,7 @@
     </row>
     <row r="64" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>10</v>
@@ -12193,61 +12196,61 @@
         <v>0</v>
       </c>
       <c r="Q64">
-        <v>0.05</v>
+        <v>-0.08</v>
       </c>
       <c r="R64">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="S64">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="T64">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="U64">
         <v>0</v>
       </c>
       <c r="V64">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="W64">
         <v>-0.2</v>
       </c>
       <c r="X64">
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
       <c r="Y64">
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
       <c r="Z64">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AA64">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AB64">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC64">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD64">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE64">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AF64">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="AG64">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="AH64">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="AI64">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AJ64">
         <v>0</v>
@@ -12264,118 +12267,118 @@
     </row>
     <row r="65" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q65">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="R65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V65">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="W65">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="X65">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="Y65">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="Z65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH65">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="AI65">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AJ65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM65" s="2" t="s">
         <v>12</v>
@@ -12383,7 +12386,7 @@
     </row>
     <row r="66" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>10</v>
@@ -12502,7 +12505,7 @@
     </row>
     <row r="67" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>10</v>
@@ -12532,88 +12535,88 @@
         <v>1</v>
       </c>
       <c r="K67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM67" s="2" t="s">
         <v>12</v>
@@ -12621,13 +12624,13 @@
     </row>
     <row r="68" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -12648,58 +12651,58 @@
         <v>1</v>
       </c>
       <c r="J68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K68">
         <v>0</v>
       </c>
       <c r="L68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB68">
         <v>0</v>
@@ -12708,10 +12711,10 @@
         <v>0</v>
       </c>
       <c r="AD68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF68">
         <v>0</v>
@@ -12720,13 +12723,13 @@
         <v>0</v>
       </c>
       <c r="AH68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK68">
         <v>0</v>
@@ -12740,7 +12743,7 @@
     </row>
     <row r="69" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>10</v>
@@ -12749,22 +12752,22 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J69">
         <v>0</v>
@@ -12773,79 +12776,79 @@
         <v>0</v>
       </c>
       <c r="L69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q69">
-        <v>-0.08</v>
+        <v>1</v>
       </c>
       <c r="R69">
-        <v>-0.1</v>
+        <v>1</v>
       </c>
       <c r="S69">
-        <v>-0.1</v>
+        <v>1</v>
       </c>
       <c r="T69">
-        <v>-0.1</v>
+        <v>1</v>
       </c>
       <c r="U69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V69">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="W69">
-        <v>-0.2</v>
+        <v>1</v>
       </c>
       <c r="X69">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y69">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z69">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AA69">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AB69">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC69">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD69">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AE69">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AF69">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AG69">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AH69">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="AI69">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AJ69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK69">
         <v>0</v>
@@ -12859,7 +12862,7 @@
     </row>
     <row r="70" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>10</v>
@@ -12907,61 +12910,61 @@
         <v>0</v>
       </c>
       <c r="Q70">
-        <v>0.05</v>
+        <v>-0.08</v>
       </c>
       <c r="R70">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="S70">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="T70">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="U70">
         <v>0</v>
       </c>
       <c r="V70">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="W70">
         <v>-0.2</v>
       </c>
       <c r="X70">
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
       <c r="Y70">
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
       <c r="Z70">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AA70">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AB70">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC70">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD70">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE70">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AF70">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="AG70">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="AH70">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="AI70">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AJ70">
         <v>0</v>
@@ -12978,118 +12981,118 @@
     </row>
     <row r="71" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q71">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="R71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V71">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="W71">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="X71">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="Y71">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="Z71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH71">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="AI71">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AJ71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM71" s="2" t="s">
         <v>12</v>
@@ -13097,7 +13100,7 @@
     </row>
     <row r="72" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>10</v>
@@ -13216,7 +13219,7 @@
     </row>
     <row r="73" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>10</v>
@@ -13246,88 +13249,88 @@
         <v>1</v>
       </c>
       <c r="K73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM73" s="2" t="s">
         <v>12</v>
@@ -13335,13 +13338,13 @@
     </row>
     <row r="74" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -13365,88 +13368,88 @@
         <v>1</v>
       </c>
       <c r="K74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W74">
         <v>0</v>
       </c>
       <c r="X74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM74" s="2" t="s">
         <v>12</v>
@@ -13454,7 +13457,7 @@
     </row>
     <row r="75" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>10</v>
@@ -13463,109 +13466,109 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E75">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F75">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="G75">
         <v>1</v>
       </c>
       <c r="H75">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I75">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J75">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="K75">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="L75">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q75">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="R75">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="S75">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="T75">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="U75">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="V75">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="W75">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="X75">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Y75">
         <v>1</v>
       </c>
       <c r="Z75">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AA75">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AB75">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="AC75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE75">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AF75">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="AG75">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="AH75">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AI75">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="AJ75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM75" s="2" t="s">
         <v>12</v>
@@ -13573,7 +13576,7 @@
     </row>
     <row r="76" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>10</v>
@@ -13582,109 +13585,109 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F76">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="G76">
         <v>1</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I76">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="J76">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="K76">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="L76">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q76">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="R76">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="S76">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="T76">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="U76">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="V76">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="W76">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="X76">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="Y76">
         <v>1</v>
       </c>
       <c r="Z76">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="AA76">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="AB76">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AC76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE76">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="AF76">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="AG76">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AH76">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="AI76">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AJ76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM76" s="2" t="s">
         <v>12</v>
@@ -13692,7 +13695,7 @@
     </row>
     <row r="77" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>10</v>
@@ -13701,117 +13704,236 @@
         <v>0</v>
       </c>
       <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
+        <v>1</v>
+      </c>
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="M77">
+        <v>1</v>
+      </c>
+      <c r="N77">
+        <v>1</v>
+      </c>
+      <c r="O77">
+        <v>1</v>
+      </c>
+      <c r="P77">
+        <v>1</v>
+      </c>
+      <c r="Q77">
+        <v>1</v>
+      </c>
+      <c r="R77">
+        <v>1</v>
+      </c>
+      <c r="S77">
+        <v>1</v>
+      </c>
+      <c r="T77">
+        <v>1</v>
+      </c>
+      <c r="U77">
+        <v>1</v>
+      </c>
+      <c r="V77">
+        <v>1</v>
+      </c>
+      <c r="W77">
+        <v>0</v>
+      </c>
+      <c r="X77">
+        <v>1</v>
+      </c>
+      <c r="Y77">
+        <v>1</v>
+      </c>
+      <c r="Z77">
+        <v>1</v>
+      </c>
+      <c r="AA77">
+        <v>1</v>
+      </c>
+      <c r="AB77">
+        <v>1</v>
+      </c>
+      <c r="AC77">
+        <v>1</v>
+      </c>
+      <c r="AD77">
+        <v>1</v>
+      </c>
+      <c r="AE77">
+        <v>1</v>
+      </c>
+      <c r="AF77">
+        <v>1</v>
+      </c>
+      <c r="AG77">
+        <v>1</v>
+      </c>
+      <c r="AH77">
+        <v>1</v>
+      </c>
+      <c r="AI77">
+        <v>1</v>
+      </c>
+      <c r="AJ77">
+        <v>1</v>
+      </c>
+      <c r="AK77">
+        <v>1</v>
+      </c>
+      <c r="AL77">
+        <v>1</v>
+      </c>
+      <c r="AM77" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
         <v>0.05</v>
       </c>
-      <c r="E77">
+      <c r="E78">
         <v>0.3</v>
       </c>
-      <c r="F77">
+      <c r="F78">
         <v>0.7</v>
       </c>
-      <c r="G77">
-        <v>1</v>
-      </c>
-      <c r="H77">
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
         <v>0.5</v>
       </c>
-      <c r="I77">
+      <c r="I78">
         <v>0.7</v>
       </c>
-      <c r="J77">
+      <c r="J78">
         <v>0.7</v>
       </c>
-      <c r="K77">
+      <c r="K78">
         <v>0.3</v>
       </c>
-      <c r="L77">
+      <c r="L78">
         <v>0.1</v>
       </c>
-      <c r="M77">
-        <v>0</v>
-      </c>
-      <c r="N77">
-        <v>0</v>
-      </c>
-      <c r="O77">
-        <v>0</v>
-      </c>
-      <c r="P77">
-        <v>0</v>
-      </c>
-      <c r="Q77">
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="N78">
+        <v>0</v>
+      </c>
+      <c r="O78">
+        <v>0</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
         <v>0.3</v>
       </c>
-      <c r="R77">
+      <c r="R78">
         <v>0.4</v>
       </c>
-      <c r="S77">
+      <c r="S78">
         <v>0.1</v>
       </c>
-      <c r="T77">
+      <c r="T78">
         <v>0.1</v>
       </c>
-      <c r="U77">
+      <c r="U78">
         <v>0.1</v>
       </c>
-      <c r="V77">
+      <c r="V78">
         <v>0.2</v>
       </c>
-      <c r="W77">
+      <c r="W78">
         <v>0.3</v>
       </c>
-      <c r="X77">
+      <c r="X78">
         <v>0.4</v>
       </c>
-      <c r="Y77">
-        <v>1</v>
-      </c>
-      <c r="Z77">
+      <c r="Y78">
+        <v>1</v>
+      </c>
+      <c r="Z78">
         <v>0.4</v>
       </c>
-      <c r="AA77">
+      <c r="AA78">
         <v>0.3</v>
       </c>
-      <c r="AB77">
+      <c r="AB78">
         <v>0.1</v>
       </c>
-      <c r="AC77">
-        <v>0</v>
-      </c>
-      <c r="AD77">
-        <v>0</v>
-      </c>
-      <c r="AE77">
+      <c r="AC78">
+        <v>0</v>
+      </c>
+      <c r="AD78">
+        <v>0</v>
+      </c>
+      <c r="AE78">
         <v>0.3</v>
       </c>
-      <c r="AF77">
+      <c r="AF78">
         <v>0.6</v>
       </c>
-      <c r="AG77">
+      <c r="AG78">
         <v>0.1</v>
       </c>
-      <c r="AH77">
+      <c r="AH78">
         <v>0.2</v>
       </c>
-      <c r="AI77">
+      <c r="AI78">
         <v>0.1</v>
       </c>
-      <c r="AJ77">
-        <v>0</v>
-      </c>
-      <c r="AK77">
-        <v>0</v>
-      </c>
-      <c r="AL77">
-        <v>0</v>
-      </c>
-      <c r="AM77" s="2" t="s">
+      <c r="AJ78">
+        <v>0</v>
+      </c>
+      <c r="AK78">
+        <v>0</v>
+      </c>
+      <c r="AL78">
+        <v>0</v>
+      </c>
+      <c r="AM78" s="2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C9:AL9">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13822,7 +13944,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C68:AL68">
+  <conditionalFormatting sqref="C69:AL69">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:AL9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -13834,20 +13968,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:AL9">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C69:AL70">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="C70:AL71">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13857,7 +13979,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:AL8">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13866,8 +13988,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:AL61">
-    <cfRule type="colorScale" priority="20">
+  <conditionalFormatting sqref="C11:AL55 C57:AL62">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13879,7 +14001,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:AL10">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13891,7 +14013,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:AL3">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13903,7 +14025,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:AL3">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13915,7 +14037,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:AL2">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13925,7 +14047,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:AL4">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13937,7 +14059,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:AL6">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13949,6 +14071,40 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:AL6">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:AL5">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:AL7">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:AL63">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -13960,8 +14116,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:AL5">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="C64:AL65">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13970,20 +14126,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:AL7">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62:AL62">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="C77:AL78">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13994,17 +14138,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63:AL64">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="C75:AL75">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76:AL77">
+  <conditionalFormatting sqref="C76:AL76">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -14016,27 +14162,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C74:AL74">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C75:AL75">
+  <conditionalFormatting sqref="C56:AL56">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>